<commit_message>
Add uncharged gem and altar classes, add altar statics recolors
</commit_message>
<xml_diff>
--- a/server/Dungeonz.io translations.xlsx
+++ b/server/Dungeonz.io translations.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="1577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="1581">
   <si>
     <t>Dungeonz.io translations</t>
   </si>
@@ -3528,6 +3528,18 @@
   </si>
   <si>
     <t>一件快速的中程武器。</t>
+  </si>
+  <si>
+    <t>Item name: Gem</t>
+  </si>
+  <si>
+    <t>Gem</t>
+  </si>
+  <si>
+    <t>Item description: Gem</t>
+  </si>
+  <si>
+    <t>Can be charged at a magic altar using glory to add an elemental effect.</t>
   </si>
   <si>
     <t>Item name: Fire gem</t>
@@ -19880,20 +19892,16 @@
         <v>1170</v>
       </c>
       <c r="C374" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B374, ""en"", ""fr"")"),"petit bijou d'incendie")</f>
-        <v>petit bijou d'incendie</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B374, ""en"", ""fr"")"),"Gemme")</f>
+        <v>Gemme</v>
       </c>
       <c r="D374" s="23"/>
       <c r="E374" s="29"/>
-      <c r="F374" s="23" t="s">
-        <v>1171</v>
-      </c>
+      <c r="F374" s="23"/>
       <c r="G374" s="29"/>
       <c r="H374" s="36"/>
       <c r="I374" s="29"/>
-      <c r="J374" s="25" t="s">
-        <v>1172</v>
-      </c>
+      <c r="J374" s="25"/>
       <c r="K374" s="30"/>
       <c r="L374" s="35"/>
       <c r="M374" s="28"/>
@@ -19915,26 +19923,22 @@
     </row>
     <row r="375">
       <c r="A375" s="21" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="B375" s="22" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="C375" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B375, ""en"", ""fr"")"),"Utilisé pour des objets d'artisanat avec un effet de feu.")</f>
-        <v>Utilisé pour des objets d'artisanat avec un effet de feu.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B375, ""en"", ""fr"")"),"Peut être chargé à un autel magique en utilisant la gloire d'ajouter un effet élémentaire.")</f>
+        <v>Peut être chargé à un autel magique en utilisant la gloire d'ajouter un effet élémentaire.</v>
       </c>
       <c r="D375" s="23"/>
       <c r="E375" s="29"/>
-      <c r="F375" s="23" t="s">
-        <v>1175</v>
-      </c>
+      <c r="F375" s="23"/>
       <c r="G375" s="29"/>
       <c r="H375" s="36"/>
       <c r="I375" s="29"/>
-      <c r="J375" s="25" t="s">
-        <v>1176</v>
-      </c>
+      <c r="J375" s="25"/>
       <c r="K375" s="30"/>
       <c r="L375" s="35"/>
       <c r="M375" s="28"/>
@@ -19956,25 +19960,25 @@
     </row>
     <row r="376">
       <c r="A376" s="21" t="s">
-        <v>1177</v>
+        <v>1173</v>
       </c>
       <c r="B376" s="22" t="s">
-        <v>1178</v>
+        <v>1174</v>
       </c>
       <c r="C376" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B376, ""en"", ""fr"")"),"joyau du vent")</f>
-        <v>joyau du vent</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B376, ""en"", ""fr"")"),"petit bijou d'incendie")</f>
+        <v>petit bijou d'incendie</v>
       </c>
       <c r="D376" s="23"/>
       <c r="E376" s="29"/>
       <c r="F376" s="23" t="s">
-        <v>1179</v>
+        <v>1175</v>
       </c>
       <c r="G376" s="29"/>
       <c r="H376" s="36"/>
       <c r="I376" s="29"/>
       <c r="J376" s="25" t="s">
-        <v>1180</v>
+        <v>1176</v>
       </c>
       <c r="K376" s="30"/>
       <c r="L376" s="35"/>
@@ -19997,25 +20001,25 @@
     </row>
     <row r="377">
       <c r="A377" s="21" t="s">
-        <v>1181</v>
+        <v>1177</v>
       </c>
       <c r="B377" s="22" t="s">
-        <v>1182</v>
+        <v>1178</v>
       </c>
       <c r="C377" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B377, ""en"", ""fr"")"),"Utilisé pour des objets d'artisanat avec un effet du vent.")</f>
-        <v>Utilisé pour des objets d'artisanat avec un effet du vent.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B377, ""en"", ""fr"")"),"Utilisé pour des objets d'artisanat avec un effet de feu.")</f>
+        <v>Utilisé pour des objets d'artisanat avec un effet de feu.</v>
       </c>
       <c r="D377" s="23"/>
       <c r="E377" s="29"/>
       <c r="F377" s="23" t="s">
-        <v>1183</v>
+        <v>1179</v>
       </c>
       <c r="G377" s="29"/>
       <c r="H377" s="36"/>
       <c r="I377" s="29"/>
       <c r="J377" s="25" t="s">
-        <v>1184</v>
+        <v>1180</v>
       </c>
       <c r="K377" s="30"/>
       <c r="L377" s="35"/>
@@ -20038,25 +20042,25 @@
     </row>
     <row r="378">
       <c r="A378" s="21" t="s">
-        <v>1185</v>
+        <v>1181</v>
       </c>
       <c r="B378" s="22" t="s">
-        <v>1186</v>
+        <v>1182</v>
       </c>
       <c r="C378" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B378, ""en"", ""fr"")"),"petit bijou de sang")</f>
-        <v>petit bijou de sang</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B378, ""en"", ""fr"")"),"joyau du vent")</f>
+        <v>joyau du vent</v>
       </c>
       <c r="D378" s="23"/>
       <c r="E378" s="29"/>
       <c r="F378" s="23" t="s">
-        <v>1187</v>
+        <v>1183</v>
       </c>
       <c r="G378" s="29"/>
       <c r="H378" s="36"/>
       <c r="I378" s="29"/>
       <c r="J378" s="25" t="s">
-        <v>1188</v>
+        <v>1184</v>
       </c>
       <c r="K378" s="30"/>
       <c r="L378" s="35"/>
@@ -20079,25 +20083,25 @@
     </row>
     <row r="379">
       <c r="A379" s="21" t="s">
-        <v>1189</v>
+        <v>1185</v>
       </c>
       <c r="B379" s="22" t="s">
-        <v>1190</v>
+        <v>1186</v>
       </c>
       <c r="C379" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B379, ""en"", ""fr"")"),"Utilisé pour des objets d'artisanat avec un effet lifesteal.")</f>
-        <v>Utilisé pour des objets d'artisanat avec un effet lifesteal.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B379, ""en"", ""fr"")"),"Utilisé pour des objets d'artisanat avec un effet du vent.")</f>
+        <v>Utilisé pour des objets d'artisanat avec un effet du vent.</v>
       </c>
       <c r="D379" s="23"/>
       <c r="E379" s="29"/>
       <c r="F379" s="23" t="s">
-        <v>1191</v>
+        <v>1187</v>
       </c>
       <c r="G379" s="29"/>
       <c r="H379" s="36"/>
       <c r="I379" s="29"/>
       <c r="J379" s="25" t="s">
-        <v>1192</v>
+        <v>1188</v>
       </c>
       <c r="K379" s="30"/>
       <c r="L379" s="35"/>
@@ -20120,25 +20124,25 @@
     </row>
     <row r="380">
       <c r="A380" s="21" t="s">
-        <v>1193</v>
+        <v>1189</v>
       </c>
       <c r="B380" s="22" t="s">
-        <v>1194</v>
+        <v>1190</v>
       </c>
       <c r="C380" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B380, ""en"", ""fr"")"),"Le personnel d'incendie")</f>
-        <v>Le personnel d'incendie</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B380, ""en"", ""fr"")"),"petit bijou de sang")</f>
+        <v>petit bijou de sang</v>
       </c>
       <c r="D380" s="23"/>
       <c r="E380" s="29"/>
       <c r="F380" s="23" t="s">
-        <v>1195</v>
+        <v>1191</v>
       </c>
       <c r="G380" s="29"/>
       <c r="H380" s="36"/>
       <c r="I380" s="29"/>
       <c r="J380" s="25" t="s">
-        <v>1196</v>
+        <v>1192</v>
       </c>
       <c r="K380" s="30"/>
       <c r="L380" s="35"/>
@@ -20161,25 +20165,25 @@
     </row>
     <row r="381">
       <c r="A381" s="21" t="s">
-        <v>1197</v>
+        <v>1193</v>
       </c>
       <c r="B381" s="22" t="s">
-        <v>1198</v>
+        <v>1194</v>
       </c>
       <c r="C381" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B381, ""en"", ""fr"")"),"Shoots feu qui inflige des blessures.")</f>
-        <v>Shoots feu qui inflige des blessures.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B381, ""en"", ""fr"")"),"Utilisé pour des objets d'artisanat avec un effet lifesteal.")</f>
+        <v>Utilisé pour des objets d'artisanat avec un effet lifesteal.</v>
       </c>
       <c r="D381" s="23"/>
       <c r="E381" s="29"/>
       <c r="F381" s="23" t="s">
-        <v>1199</v>
+        <v>1195</v>
       </c>
       <c r="G381" s="29"/>
       <c r="H381" s="36"/>
       <c r="I381" s="29"/>
       <c r="J381" s="25" t="s">
-        <v>1200</v>
+        <v>1196</v>
       </c>
       <c r="K381" s="30"/>
       <c r="L381" s="35"/>
@@ -20202,25 +20206,25 @@
     </row>
     <row r="382">
       <c r="A382" s="21" t="s">
-        <v>1201</v>
+        <v>1197</v>
       </c>
       <c r="B382" s="22" t="s">
-        <v>1202</v>
+        <v>1198</v>
       </c>
       <c r="C382" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B382, ""en"", ""fr"")"),"Super personnel d'incendie")</f>
-        <v>Super personnel d'incendie</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B382, ""en"", ""fr"")"),"Le personnel d'incendie")</f>
+        <v>Le personnel d'incendie</v>
       </c>
       <c r="D382" s="23"/>
       <c r="E382" s="29"/>
       <c r="F382" s="23" t="s">
-        <v>1203</v>
+        <v>1199</v>
       </c>
       <c r="G382" s="29"/>
       <c r="H382" s="36"/>
       <c r="I382" s="29"/>
       <c r="J382" s="25" t="s">
-        <v>1204</v>
+        <v>1200</v>
       </c>
       <c r="K382" s="30"/>
       <c r="L382" s="35"/>
@@ -20243,25 +20247,25 @@
     </row>
     <row r="383">
       <c r="A383" s="21" t="s">
-        <v>1205</v>
+        <v>1201</v>
       </c>
       <c r="B383" s="22" t="s">
-        <v>1206</v>
+        <v>1202</v>
       </c>
       <c r="C383" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B383, ""en"", ""fr"")"),"Shoots feu qui tire plus de feu.")</f>
-        <v>Shoots feu qui tire plus de feu.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B383, ""en"", ""fr"")"),"Shoots feu qui inflige des blessures.")</f>
+        <v>Shoots feu qui inflige des blessures.</v>
       </c>
       <c r="D383" s="23"/>
       <c r="E383" s="29"/>
       <c r="F383" s="23" t="s">
-        <v>1207</v>
+        <v>1203</v>
       </c>
       <c r="G383" s="29"/>
       <c r="H383" s="36"/>
       <c r="I383" s="29"/>
       <c r="J383" s="25" t="s">
-        <v>1208</v>
+        <v>1204</v>
       </c>
       <c r="K383" s="30"/>
       <c r="L383" s="35"/>
@@ -20284,25 +20288,25 @@
     </row>
     <row r="384">
       <c r="A384" s="21" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
       <c r="B384" s="22" t="s">
-        <v>1210</v>
+        <v>1206</v>
       </c>
       <c r="C384" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B384, ""en"", ""fr"")"),"Le personnel du vent")</f>
-        <v>Le personnel du vent</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B384, ""en"", ""fr"")"),"Super personnel d'incendie")</f>
+        <v>Super personnel d'incendie</v>
       </c>
       <c r="D384" s="23"/>
       <c r="E384" s="29"/>
       <c r="F384" s="23" t="s">
-        <v>1211</v>
+        <v>1207</v>
       </c>
       <c r="G384" s="29"/>
       <c r="H384" s="36"/>
       <c r="I384" s="29"/>
       <c r="J384" s="25" t="s">
-        <v>1212</v>
+        <v>1208</v>
       </c>
       <c r="K384" s="30"/>
       <c r="L384" s="35"/>
@@ -20325,25 +20329,25 @@
     </row>
     <row r="385">
       <c r="A385" s="21" t="s">
-        <v>1213</v>
+        <v>1209</v>
       </c>
       <c r="B385" s="22" t="s">
-        <v>1214</v>
+        <v>1210</v>
       </c>
       <c r="C385" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B385, ""en"", ""fr"")"),"Shoots vent qui frappe les choses.")</f>
-        <v>Shoots vent qui frappe les choses.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B385, ""en"", ""fr"")"),"Shoots feu qui tire plus de feu.")</f>
+        <v>Shoots feu qui tire plus de feu.</v>
       </c>
       <c r="D385" s="23"/>
       <c r="E385" s="29"/>
       <c r="F385" s="23" t="s">
-        <v>1215</v>
+        <v>1211</v>
       </c>
       <c r="G385" s="29"/>
       <c r="H385" s="36"/>
       <c r="I385" s="29"/>
       <c r="J385" s="25" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="K385" s="30"/>
       <c r="L385" s="35"/>
@@ -20366,25 +20370,25 @@
     </row>
     <row r="386">
       <c r="A386" s="21" t="s">
-        <v>1217</v>
+        <v>1213</v>
       </c>
       <c r="B386" s="22" t="s">
-        <v>1218</v>
+        <v>1214</v>
       </c>
       <c r="C386" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B386, ""en"", ""fr"")"),"Super personnel du vent")</f>
-        <v>Super personnel du vent</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B386, ""en"", ""fr"")"),"Le personnel du vent")</f>
+        <v>Le personnel du vent</v>
       </c>
       <c r="D386" s="23"/>
       <c r="E386" s="29"/>
       <c r="F386" s="23" t="s">
-        <v>1219</v>
+        <v>1215</v>
       </c>
       <c r="G386" s="29"/>
       <c r="H386" s="36"/>
       <c r="I386" s="29"/>
       <c r="J386" s="25" t="s">
-        <v>1220</v>
+        <v>1216</v>
       </c>
       <c r="K386" s="30"/>
       <c r="L386" s="35"/>
@@ -20407,25 +20411,25 @@
     </row>
     <row r="387">
       <c r="A387" s="21" t="s">
-        <v>1221</v>
+        <v>1217</v>
       </c>
       <c r="B387" s="22" t="s">
-        <v>1222</v>
+        <v>1218</v>
       </c>
       <c r="C387" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B387, ""en"", ""fr"")"),"Shoots vent qui tire plus de vent.")</f>
-        <v>Shoots vent qui tire plus de vent.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B387, ""en"", ""fr"")"),"Shoots vent qui frappe les choses.")</f>
+        <v>Shoots vent qui frappe les choses.</v>
       </c>
       <c r="D387" s="23"/>
       <c r="E387" s="29"/>
       <c r="F387" s="23" t="s">
-        <v>1223</v>
+        <v>1219</v>
       </c>
       <c r="G387" s="29"/>
       <c r="H387" s="36"/>
       <c r="I387" s="29"/>
       <c r="J387" s="25" t="s">
-        <v>1224</v>
+        <v>1220</v>
       </c>
       <c r="K387" s="30"/>
       <c r="L387" s="35"/>
@@ -20448,25 +20452,25 @@
     </row>
     <row r="388">
       <c r="A388" s="21" t="s">
-        <v>1225</v>
+        <v>1221</v>
       </c>
       <c r="B388" s="22" t="s">
-        <v>1226</v>
+        <v>1222</v>
       </c>
       <c r="C388" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B388, ""en"", ""fr"")"),"Le personnel de sang")</f>
-        <v>Le personnel de sang</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B388, ""en"", ""fr"")"),"Super personnel du vent")</f>
+        <v>Super personnel du vent</v>
       </c>
       <c r="D388" s="23"/>
       <c r="E388" s="29"/>
       <c r="F388" s="23" t="s">
-        <v>1227</v>
+        <v>1223</v>
       </c>
       <c r="G388" s="29"/>
       <c r="H388" s="36"/>
       <c r="I388" s="29"/>
       <c r="J388" s="25" t="s">
-        <v>1228</v>
+        <v>1224</v>
       </c>
       <c r="K388" s="30"/>
       <c r="L388" s="35"/>
@@ -20489,25 +20493,25 @@
     </row>
     <row r="389">
       <c r="A389" s="21" t="s">
-        <v>1229</v>
+        <v>1225</v>
       </c>
       <c r="B389" s="22" t="s">
-        <v>1230</v>
+        <v>1226</v>
       </c>
       <c r="C389" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B389, ""en"", ""fr"")"),"Shoots un projectile qui vole hitpoints. Consomme hitpoints lorsqu'il est utilisé.")</f>
-        <v>Shoots un projectile qui vole hitpoints. Consomme hitpoints lorsqu'il est utilisé.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B389, ""en"", ""fr"")"),"Shoots vent qui tire plus de vent.")</f>
+        <v>Shoots vent qui tire plus de vent.</v>
       </c>
       <c r="D389" s="23"/>
       <c r="E389" s="29"/>
       <c r="F389" s="23" t="s">
-        <v>1231</v>
+        <v>1227</v>
       </c>
       <c r="G389" s="29"/>
       <c r="H389" s="36"/>
       <c r="I389" s="29"/>
       <c r="J389" s="25" t="s">
-        <v>1232</v>
+        <v>1228</v>
       </c>
       <c r="K389" s="30"/>
       <c r="L389" s="35"/>
@@ -20530,25 +20534,25 @@
     </row>
     <row r="390">
       <c r="A390" s="21" t="s">
-        <v>1233</v>
+        <v>1229</v>
       </c>
       <c r="B390" s="22" t="s">
-        <v>1234</v>
+        <v>1230</v>
       </c>
       <c r="C390" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B390, ""en"", ""fr"")"),"Super personnel de sang")</f>
-        <v>Super personnel de sang</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B390, ""en"", ""fr"")"),"Le personnel de sang")</f>
+        <v>Le personnel de sang</v>
       </c>
       <c r="D390" s="23"/>
       <c r="E390" s="29"/>
       <c r="F390" s="23" t="s">
-        <v>1235</v>
+        <v>1231</v>
       </c>
       <c r="G390" s="29"/>
       <c r="H390" s="36"/>
       <c r="I390" s="29"/>
       <c r="J390" s="25" t="s">
-        <v>1236</v>
+        <v>1232</v>
       </c>
       <c r="K390" s="30"/>
       <c r="L390" s="35"/>
@@ -20571,25 +20575,25 @@
     </row>
     <row r="391">
       <c r="A391" s="21" t="s">
-        <v>1237</v>
+        <v>1233</v>
       </c>
       <c r="B391" s="22" t="s">
-        <v>1238</v>
+        <v>1234</v>
       </c>
       <c r="C391" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B391, ""en"", ""fr"")"),"Shoots un projectile qui tire des projectiles lifesteal plus lifesteal.")</f>
-        <v>Shoots un projectile qui tire des projectiles lifesteal plus lifesteal.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B391, ""en"", ""fr"")"),"Shoots un projectile qui vole hitpoints. Consomme hitpoints lorsqu'il est utilisé.")</f>
+        <v>Shoots un projectile qui vole hitpoints. Consomme hitpoints lorsqu'il est utilisé.</v>
       </c>
       <c r="D391" s="23"/>
       <c r="E391" s="29"/>
       <c r="F391" s="23" t="s">
-        <v>1239</v>
+        <v>1235</v>
       </c>
       <c r="G391" s="29"/>
       <c r="H391" s="36"/>
       <c r="I391" s="29"/>
       <c r="J391" s="25" t="s">
-        <v>1240</v>
+        <v>1236</v>
       </c>
       <c r="K391" s="30"/>
       <c r="L391" s="35"/>
@@ -20612,25 +20616,25 @@
     </row>
     <row r="392">
       <c r="A392" s="21" t="s">
-        <v>1241</v>
+        <v>1237</v>
       </c>
       <c r="B392" s="22" t="s">
-        <v>1242</v>
+        <v>1238</v>
       </c>
       <c r="C392" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B392, ""en"", ""fr"")"),"Livre de lumière")</f>
-        <v>Livre de lumière</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B392, ""en"", ""fr"")"),"Super personnel de sang")</f>
+        <v>Super personnel de sang</v>
       </c>
       <c r="D392" s="23"/>
       <c r="E392" s="29"/>
       <c r="F392" s="23" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
       <c r="G392" s="29"/>
       <c r="H392" s="36"/>
       <c r="I392" s="29"/>
       <c r="J392" s="25" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
       <c r="K392" s="30"/>
       <c r="L392" s="35"/>
@@ -20653,25 +20657,25 @@
     </row>
     <row r="393">
       <c r="A393" s="21" t="s">
-        <v>1245</v>
+        <v>1241</v>
       </c>
       <c r="B393" s="22" t="s">
-        <v>1246</v>
+        <v>1242</v>
       </c>
       <c r="C393" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B393, ""en"", ""fr"")"),"Un livre de sorts de soutien.")</f>
-        <v>Un livre de sorts de soutien.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B393, ""en"", ""fr"")"),"Shoots un projectile qui tire des projectiles lifesteal plus lifesteal.")</f>
+        <v>Shoots un projectile qui tire des projectiles lifesteal plus lifesteal.</v>
       </c>
       <c r="D393" s="23"/>
       <c r="E393" s="29"/>
       <c r="F393" s="23" t="s">
-        <v>1247</v>
+        <v>1243</v>
       </c>
       <c r="G393" s="29"/>
       <c r="H393" s="36"/>
       <c r="I393" s="29"/>
       <c r="J393" s="25" t="s">
-        <v>1248</v>
+        <v>1244</v>
       </c>
       <c r="K393" s="30"/>
       <c r="L393" s="35"/>
@@ -20694,25 +20698,25 @@
     </row>
     <row r="394">
       <c r="A394" s="21" t="s">
-        <v>1249</v>
+        <v>1245</v>
       </c>
       <c r="B394" s="22" t="s">
-        <v>1250</v>
+        <v>1246</v>
       </c>
       <c r="C394" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B394, ""en"", ""fr"")"),"Livre des âmes")</f>
-        <v>Livre des âmes</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B394, ""en"", ""fr"")"),"Livre de lumière")</f>
+        <v>Livre de lumière</v>
       </c>
       <c r="D394" s="23"/>
       <c r="E394" s="29"/>
       <c r="F394" s="23" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
       <c r="G394" s="29"/>
       <c r="H394" s="36"/>
       <c r="I394" s="29"/>
       <c r="J394" s="25" t="s">
-        <v>1252</v>
+        <v>1248</v>
       </c>
       <c r="K394" s="30"/>
       <c r="L394" s="35"/>
@@ -20735,25 +20739,25 @@
     </row>
     <row r="395">
       <c r="A395" s="21" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
       <c r="B395" s="22" t="s">
-        <v>1254</v>
+        <v>1250</v>
       </c>
       <c r="C395" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B395, ""en"", ""fr"")"),"Un livre de sorts d'invocation.")</f>
-        <v>Un livre de sorts d'invocation.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B395, ""en"", ""fr"")"),"Un livre de sorts de soutien.")</f>
+        <v>Un livre de sorts de soutien.</v>
       </c>
       <c r="D395" s="23"/>
       <c r="E395" s="29"/>
       <c r="F395" s="23" t="s">
-        <v>1255</v>
+        <v>1251</v>
       </c>
       <c r="G395" s="29"/>
       <c r="H395" s="36"/>
       <c r="I395" s="29"/>
       <c r="J395" s="25" t="s">
-        <v>1256</v>
+        <v>1252</v>
       </c>
       <c r="K395" s="30"/>
       <c r="L395" s="35"/>
@@ -20776,27 +20780,25 @@
     </row>
     <row r="396">
       <c r="A396" s="21" t="s">
-        <v>1257</v>
+        <v>1253</v>
       </c>
       <c r="B396" s="22" t="s">
-        <v>1258</v>
+        <v>1254</v>
       </c>
       <c r="C396" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B396, ""en"", ""fr"")"),"flèches d'os")</f>
-        <v>flèches d'os</v>
-      </c>
-      <c r="D396" s="23" t="s">
-        <v>1259</v>
-      </c>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B396, ""en"", ""fr"")"),"Livre des âmes")</f>
+        <v>Livre des âmes</v>
+      </c>
+      <c r="D396" s="23"/>
       <c r="E396" s="29"/>
       <c r="F396" s="23" t="s">
-        <v>1260</v>
+        <v>1255</v>
       </c>
       <c r="G396" s="29"/>
       <c r="H396" s="36"/>
       <c r="I396" s="29"/>
       <c r="J396" s="25" t="s">
-        <v>1261</v>
+        <v>1256</v>
       </c>
       <c r="K396" s="30"/>
       <c r="L396" s="35"/>
@@ -20819,27 +20821,25 @@
     </row>
     <row r="397">
       <c r="A397" s="21" t="s">
-        <v>1262</v>
+        <v>1257</v>
       </c>
       <c r="B397" s="22" t="s">
-        <v>1031</v>
+        <v>1258</v>
       </c>
       <c r="C397" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B397, ""en"", ""fr"")"),"Utilisé comme munitions pour un arc.")</f>
-        <v>Utilisé comme munitions pour un arc.</v>
-      </c>
-      <c r="D397" s="23" t="s">
-        <v>1263</v>
-      </c>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B397, ""en"", ""fr"")"),"Un livre de sorts d'invocation.")</f>
+        <v>Un livre de sorts d'invocation.</v>
+      </c>
+      <c r="D397" s="23"/>
       <c r="E397" s="29"/>
       <c r="F397" s="23" t="s">
-        <v>1078</v>
+        <v>1259</v>
       </c>
       <c r="G397" s="29"/>
       <c r="H397" s="36"/>
       <c r="I397" s="29"/>
       <c r="J397" s="25" t="s">
-        <v>1264</v>
+        <v>1260</v>
       </c>
       <c r="K397" s="30"/>
       <c r="L397" s="35"/>
@@ -20862,25 +20862,27 @@
     </row>
     <row r="398">
       <c r="A398" s="21" t="s">
-        <v>1265</v>
+        <v>1261</v>
       </c>
       <c r="B398" s="22" t="s">
-        <v>1266</v>
+        <v>1262</v>
       </c>
       <c r="C398" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B398, ""en"", ""fr"")"),"Peignoir")</f>
-        <v>Peignoir</v>
-      </c>
-      <c r="D398" s="23"/>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B398, ""en"", ""fr"")"),"flèches d'os")</f>
+        <v>flèches d'os</v>
+      </c>
+      <c r="D398" s="23" t="s">
+        <v>1263</v>
+      </c>
       <c r="E398" s="29"/>
       <c r="F398" s="23" t="s">
-        <v>1267</v>
+        <v>1264</v>
       </c>
       <c r="G398" s="29"/>
       <c r="H398" s="36"/>
       <c r="I398" s="29"/>
       <c r="J398" s="25" t="s">
-        <v>1268</v>
+        <v>1265</v>
       </c>
       <c r="K398" s="30"/>
       <c r="L398" s="35"/>
@@ -20903,25 +20905,27 @@
     </row>
     <row r="399">
       <c r="A399" s="21" t="s">
-        <v>1269</v>
+        <v>1266</v>
       </c>
       <c r="B399" s="22" t="s">
-        <v>1270</v>
+        <v>1031</v>
       </c>
       <c r="C399" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B399, ""en"", ""fr"")"),"Une robe simple. Augmente votre Potionry stat alors porté.")</f>
-        <v>Une robe simple. Augmente votre Potionry stat alors porté.</v>
-      </c>
-      <c r="D399" s="23"/>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B399, ""en"", ""fr"")"),"Utilisé comme munitions pour un arc.")</f>
+        <v>Utilisé comme munitions pour un arc.</v>
+      </c>
+      <c r="D399" s="23" t="s">
+        <v>1267</v>
+      </c>
       <c r="E399" s="29"/>
       <c r="F399" s="23" t="s">
-        <v>1271</v>
+        <v>1078</v>
       </c>
       <c r="G399" s="29"/>
       <c r="H399" s="36"/>
       <c r="I399" s="29"/>
       <c r="J399" s="25" t="s">
-        <v>1272</v>
+        <v>1268</v>
       </c>
       <c r="K399" s="30"/>
       <c r="L399" s="35"/>
@@ -20944,25 +20948,25 @@
     </row>
     <row r="400">
       <c r="A400" s="21" t="s">
-        <v>1273</v>
+        <v>1269</v>
       </c>
       <c r="B400" s="22" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
       <c r="C400" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B400, ""en"", ""fr"")"),"robe Mage")</f>
-        <v>robe Mage</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B400, ""en"", ""fr"")"),"Peignoir")</f>
+        <v>Peignoir</v>
       </c>
       <c r="D400" s="23"/>
       <c r="E400" s="29"/>
       <c r="F400" s="23" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
       <c r="G400" s="29"/>
       <c r="H400" s="36"/>
       <c r="I400" s="29"/>
       <c r="J400" s="25" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="K400" s="30"/>
       <c r="L400" s="35"/>
@@ -20985,25 +20989,25 @@
     </row>
     <row r="401">
       <c r="A401" s="21" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="B401" s="22" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
       <c r="C401" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B401, ""en"", ""fr"")"),"Une robe de base pour faire de la magie en. Augmente votre stat magique tout porté.")</f>
-        <v>Une robe de base pour faire de la magie en. Augmente votre stat magique tout porté.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B401, ""en"", ""fr"")"),"Une robe simple. Augmente votre Potionry stat alors porté.")</f>
+        <v>Une robe simple. Augmente votre Potionry stat alors porté.</v>
       </c>
       <c r="D401" s="23"/>
       <c r="E401" s="29"/>
       <c r="F401" s="23" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="G401" s="29"/>
       <c r="H401" s="36"/>
       <c r="I401" s="29"/>
       <c r="J401" s="25" t="s">
-        <v>1280</v>
+        <v>1276</v>
       </c>
       <c r="K401" s="30"/>
       <c r="L401" s="35"/>
@@ -21026,25 +21030,25 @@
     </row>
     <row r="402">
       <c r="A402" s="21" t="s">
-        <v>1281</v>
+        <v>1277</v>
       </c>
       <c r="B402" s="22" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
       <c r="C402" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B402, ""en"", ""fr"")"),"robe nécromancien")</f>
-        <v>robe nécromancien</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B402, ""en"", ""fr"")"),"robe Mage")</f>
+        <v>robe Mage</v>
       </c>
       <c r="D402" s="23"/>
       <c r="E402" s="29"/>
       <c r="F402" s="23" t="s">
-        <v>1283</v>
+        <v>1279</v>
       </c>
       <c r="G402" s="29"/>
       <c r="H402" s="36"/>
       <c r="I402" s="29"/>
       <c r="J402" s="25" t="s">
-        <v>1284</v>
+        <v>1280</v>
       </c>
       <c r="K402" s="30"/>
       <c r="L402" s="35"/>
@@ -21067,10 +21071,10 @@
     </row>
     <row r="403">
       <c r="A403" s="21" t="s">
-        <v>1285</v>
+        <v>1281</v>
       </c>
       <c r="B403" s="22" t="s">
-        <v>1278</v>
+        <v>1282</v>
       </c>
       <c r="C403" s="23" t="str">
         <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B403, ""en"", ""fr"")"),"Une robe de base pour faire de la magie en. Augmente votre stat magique tout porté.")</f>
@@ -21079,13 +21083,13 @@
       <c r="D403" s="23"/>
       <c r="E403" s="29"/>
       <c r="F403" s="23" t="s">
-        <v>1279</v>
+        <v>1283</v>
       </c>
       <c r="G403" s="29"/>
       <c r="H403" s="36"/>
       <c r="I403" s="29"/>
       <c r="J403" s="25" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="K403" s="30"/>
       <c r="L403" s="35"/>
@@ -21108,25 +21112,25 @@
     </row>
     <row r="404">
       <c r="A404" s="21" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="B404" s="22" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="C404" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B404, ""en"", ""fr"")"),"Manteau")</f>
-        <v>Manteau</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B404, ""en"", ""fr"")"),"robe nécromancien")</f>
+        <v>robe nécromancien</v>
       </c>
       <c r="D404" s="23"/>
       <c r="E404" s="29"/>
       <c r="F404" s="23" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="G404" s="29"/>
       <c r="H404" s="36"/>
       <c r="I404" s="29"/>
       <c r="J404" s="25" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="K404" s="30"/>
       <c r="L404" s="35"/>
@@ -21149,25 +21153,25 @@
     </row>
     <row r="405">
       <c r="A405" s="21" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="B405" s="22" t="s">
-        <v>1292</v>
+        <v>1282</v>
       </c>
       <c r="C405" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B405, ""en"", ""fr"")"),"Un manteau de base pour le faire à distance. Les augmentations de votre stat tout porté à distance.")</f>
-        <v>Un manteau de base pour le faire à distance. Les augmentations de votre stat tout porté à distance.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B405, ""en"", ""fr"")"),"Une robe de base pour faire de la magie en. Augmente votre stat magique tout porté.")</f>
+        <v>Une robe de base pour faire de la magie en. Augmente votre stat magique tout porté.</v>
       </c>
       <c r="D405" s="23"/>
       <c r="E405" s="29"/>
       <c r="F405" s="23" t="s">
-        <v>1293</v>
+        <v>1283</v>
       </c>
       <c r="G405" s="29"/>
       <c r="H405" s="36"/>
       <c r="I405" s="29"/>
       <c r="J405" s="25" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
       <c r="K405" s="30"/>
       <c r="L405" s="35"/>
@@ -21190,25 +21194,25 @@
     </row>
     <row r="406">
       <c r="A406" s="21" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="B406" s="22" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="C406" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B406, ""en"", ""fr"")"),"tenue Ninja")</f>
-        <v>tenue Ninja</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B406, ""en"", ""fr"")"),"Manteau")</f>
+        <v>Manteau</v>
       </c>
       <c r="D406" s="23"/>
       <c r="E406" s="29"/>
       <c r="F406" s="23" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c r="G406" s="29"/>
       <c r="H406" s="36"/>
       <c r="I406" s="29"/>
       <c r="J406" s="25" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
       <c r="K406" s="30"/>
       <c r="L406" s="35"/>
@@ -21231,25 +21235,25 @@
     </row>
     <row r="407">
       <c r="A407" s="21" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
       <c r="B407" s="22" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
       <c r="C407" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B407, ""en"", ""fr"")"),"Augmente vos stats mêlée et à distance et cache votre nom tout porté.")</f>
-        <v>Augmente vos stats mêlée et à distance et cache votre nom tout porté.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B407, ""en"", ""fr"")"),"Un manteau de base pour le faire à distance. Les augmentations de votre stat tout porté à distance.")</f>
+        <v>Un manteau de base pour le faire à distance. Les augmentations de votre stat tout porté à distance.</v>
       </c>
       <c r="D407" s="23"/>
       <c r="E407" s="29"/>
       <c r="F407" s="23" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="G407" s="29"/>
       <c r="H407" s="36"/>
       <c r="I407" s="29"/>
       <c r="J407" s="25" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="K407" s="30"/>
       <c r="L407" s="35"/>
@@ -21272,25 +21276,25 @@
     </row>
     <row r="408">
       <c r="A408" s="21" t="s">
-        <v>1303</v>
+        <v>1299</v>
       </c>
       <c r="B408" s="22" t="s">
-        <v>1304</v>
+        <v>1300</v>
       </c>
       <c r="C408" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B408, ""en"", ""fr"")"),"Charte")</f>
-        <v>Charte</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B408, ""en"", ""fr"")"),"tenue Ninja")</f>
+        <v>tenue Ninja</v>
       </c>
       <c r="D408" s="23"/>
       <c r="E408" s="29"/>
       <c r="F408" s="23" t="s">
-        <v>1305</v>
+        <v>1301</v>
       </c>
       <c r="G408" s="29"/>
       <c r="H408" s="36"/>
       <c r="I408" s="29"/>
       <c r="J408" s="25" t="s">
-        <v>1306</v>
+        <v>1302</v>
       </c>
       <c r="K408" s="30"/>
       <c r="L408" s="35"/>
@@ -21313,25 +21317,25 @@
     </row>
     <row r="409">
       <c r="A409" s="21" t="s">
-        <v>1307</v>
+        <v>1303</v>
       </c>
       <c r="B409" s="22" t="s">
-        <v>1308</v>
+        <v>1304</v>
       </c>
       <c r="C409" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B409, ""en"", ""fr"")"),"Structure du clan. Endroit pour commencer un clan. Utilisé pour concevoir d'autres structures de clan. Si cela est détruit, le clan et toutes les structures sont également détruites.")</f>
-        <v>Structure du clan. Endroit pour commencer un clan. Utilisé pour concevoir d'autres structures de clan. Si cela est détruit, le clan et toutes les structures sont également détruites.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B409, ""en"", ""fr"")"),"Augmente vos stats mêlée et à distance et cache votre nom tout porté.")</f>
+        <v>Augmente vos stats mêlée et à distance et cache votre nom tout porté.</v>
       </c>
       <c r="D409" s="23"/>
       <c r="E409" s="29"/>
       <c r="F409" s="23" t="s">
-        <v>1309</v>
+        <v>1305</v>
       </c>
       <c r="G409" s="29"/>
       <c r="H409" s="36"/>
       <c r="I409" s="29"/>
       <c r="J409" s="25" t="s">
-        <v>1310</v>
+        <v>1306</v>
       </c>
       <c r="K409" s="30"/>
       <c r="L409" s="35"/>
@@ -21354,25 +21358,25 @@
     </row>
     <row r="410">
       <c r="A410" s="21" t="s">
-        <v>1311</v>
+        <v>1307</v>
       </c>
       <c r="B410" s="22" t="s">
-        <v>1312</v>
+        <v>1308</v>
       </c>
       <c r="C410" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B410, ""en"", ""fr"")"),"Mur de bois")</f>
-        <v>Mur de bois</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B410, ""en"", ""fr"")"),"Charte")</f>
+        <v>Charte</v>
       </c>
       <c r="D410" s="23"/>
       <c r="E410" s="29"/>
       <c r="F410" s="23" t="s">
-        <v>1313</v>
+        <v>1309</v>
       </c>
       <c r="G410" s="29"/>
       <c r="H410" s="36"/>
       <c r="I410" s="29"/>
       <c r="J410" s="25" t="s">
-        <v>1314</v>
+        <v>1310</v>
       </c>
       <c r="K410" s="30"/>
       <c r="L410" s="35"/>
@@ -21395,25 +21399,25 @@
     </row>
     <row r="411">
       <c r="A411" s="21" t="s">
-        <v>1315</v>
+        <v>1311</v>
       </c>
       <c r="B411" s="22" t="s">
-        <v>1316</v>
+        <v>1312</v>
       </c>
       <c r="C411" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B411, ""en"", ""fr"")"),"Structure du clan. A faible profondeur d'une base.")</f>
-        <v>Structure du clan. A faible profondeur d'une base.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B411, ""en"", ""fr"")"),"Structure du clan. Endroit pour commencer un clan. Utilisé pour concevoir d'autres structures de clan. Si cela est détruit, le clan et toutes les structures sont également détruites.")</f>
+        <v>Structure du clan. Endroit pour commencer un clan. Utilisé pour concevoir d'autres structures de clan. Si cela est détruit, le clan et toutes les structures sont également détruites.</v>
       </c>
       <c r="D411" s="23"/>
       <c r="E411" s="29"/>
       <c r="F411" s="23" t="s">
-        <v>1317</v>
+        <v>1313</v>
       </c>
       <c r="G411" s="29"/>
       <c r="H411" s="36"/>
       <c r="I411" s="29"/>
       <c r="J411" s="25" t="s">
-        <v>1318</v>
+        <v>1314</v>
       </c>
       <c r="K411" s="30"/>
       <c r="L411" s="35"/>
@@ -21436,25 +21440,25 @@
     </row>
     <row r="412">
       <c r="A412" s="21" t="s">
-        <v>1319</v>
+        <v>1315</v>
       </c>
       <c r="B412" s="22" t="s">
-        <v>1320</v>
+        <v>1316</v>
       </c>
       <c r="C412" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B412, ""en"", ""fr"")"),"porte en bois")</f>
-        <v>porte en bois</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B412, ""en"", ""fr"")"),"Mur de bois")</f>
+        <v>Mur de bois</v>
       </c>
       <c r="D412" s="23"/>
       <c r="E412" s="29"/>
       <c r="F412" s="23" t="s">
-        <v>1321</v>
+        <v>1317</v>
       </c>
       <c r="G412" s="29"/>
       <c r="H412" s="36"/>
       <c r="I412" s="29"/>
       <c r="J412" s="25" t="s">
-        <v>1322</v>
+        <v>1318</v>
       </c>
       <c r="K412" s="30"/>
       <c r="L412" s="35"/>
@@ -21477,25 +21481,25 @@
     </row>
     <row r="413">
       <c r="A413" s="21" t="s">
-        <v>1323</v>
+        <v>1319</v>
       </c>
       <c r="B413" s="22" t="s">
-        <v>1324</v>
+        <v>1320</v>
       </c>
       <c r="C413" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B413, ""en"", ""fr"")"),"Structure du clan. Ne peut être ouvert par les membres du clan.")</f>
-        <v>Structure du clan. Ne peut être ouvert par les membres du clan.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B413, ""en"", ""fr"")"),"Structure du clan. A faible profondeur d'une base.")</f>
+        <v>Structure du clan. A faible profondeur d'une base.</v>
       </c>
       <c r="D413" s="23"/>
       <c r="E413" s="29"/>
       <c r="F413" s="23" t="s">
-        <v>1325</v>
+        <v>1321</v>
       </c>
       <c r="G413" s="29"/>
       <c r="H413" s="36"/>
       <c r="I413" s="29"/>
       <c r="J413" s="25" t="s">
-        <v>1326</v>
+        <v>1322</v>
       </c>
       <c r="K413" s="30"/>
       <c r="L413" s="35"/>
@@ -21517,26 +21521,26 @@
       <c r="AB413" s="28"/>
     </row>
     <row r="414">
-      <c r="A414" s="41" t="s">
-        <v>1327</v>
+      <c r="A414" s="21" t="s">
+        <v>1323</v>
       </c>
       <c r="B414" s="22" t="s">
-        <v>1328</v>
+        <v>1324</v>
       </c>
       <c r="C414" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B414, ""en"", ""fr"")"),"Mur de briques")</f>
-        <v>Mur de briques</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B414, ""en"", ""fr"")"),"porte en bois")</f>
+        <v>porte en bois</v>
       </c>
       <c r="D414" s="23"/>
       <c r="E414" s="29"/>
       <c r="F414" s="23" t="s">
-        <v>1329</v>
+        <v>1325</v>
       </c>
       <c r="G414" s="29"/>
       <c r="H414" s="36"/>
       <c r="I414" s="29"/>
       <c r="J414" s="25" t="s">
-        <v>1330</v>
+        <v>1326</v>
       </c>
       <c r="K414" s="30"/>
       <c r="L414" s="35"/>
@@ -21558,26 +21562,26 @@
       <c r="AB414" s="28"/>
     </row>
     <row r="415">
-      <c r="A415" s="41" t="s">
-        <v>1331</v>
+      <c r="A415" s="21" t="s">
+        <v>1327</v>
       </c>
       <c r="B415" s="22" t="s">
-        <v>1332</v>
+        <v>1328</v>
       </c>
       <c r="C415" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B415, ""en"", ""fr"")"),"Structure du clan. Une bonne défense pour une base.")</f>
-        <v>Structure du clan. Une bonne défense pour une base.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B415, ""en"", ""fr"")"),"Structure du clan. Ne peut être ouvert par les membres du clan.")</f>
+        <v>Structure du clan. Ne peut être ouvert par les membres du clan.</v>
       </c>
       <c r="D415" s="23"/>
       <c r="E415" s="29"/>
       <c r="F415" s="23" t="s">
-        <v>1333</v>
+        <v>1329</v>
       </c>
       <c r="G415" s="29"/>
       <c r="H415" s="36"/>
       <c r="I415" s="29"/>
       <c r="J415" s="25" t="s">
-        <v>1334</v>
+        <v>1330</v>
       </c>
       <c r="K415" s="30"/>
       <c r="L415" s="35"/>
@@ -21600,25 +21604,25 @@
     </row>
     <row r="416">
       <c r="A416" s="41" t="s">
-        <v>1335</v>
+        <v>1331</v>
       </c>
       <c r="B416" s="22" t="s">
-        <v>1336</v>
+        <v>1332</v>
       </c>
       <c r="C416" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B416, ""en"", ""fr"")"),"porte brique")</f>
-        <v>porte brique</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B416, ""en"", ""fr"")"),"Mur de briques")</f>
+        <v>Mur de briques</v>
       </c>
       <c r="D416" s="23"/>
       <c r="E416" s="29"/>
       <c r="F416" s="23" t="s">
-        <v>1337</v>
+        <v>1333</v>
       </c>
       <c r="G416" s="29"/>
       <c r="H416" s="36"/>
       <c r="I416" s="29"/>
       <c r="J416" s="25" t="s">
-        <v>1338</v>
+        <v>1334</v>
       </c>
       <c r="K416" s="30"/>
       <c r="L416" s="35"/>
@@ -21641,25 +21645,25 @@
     </row>
     <row r="417">
       <c r="A417" s="41" t="s">
-        <v>1339</v>
+        <v>1335</v>
       </c>
       <c r="B417" s="22" t="s">
-        <v>1340</v>
+        <v>1336</v>
       </c>
       <c r="C417" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B417, ""en"", ""fr"")"),"Structure du clan. Ne peut être ouvert par les membres du clan. Plus fort que une porte en bois.")</f>
-        <v>Structure du clan. Ne peut être ouvert par les membres du clan. Plus fort que une porte en bois.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B417, ""en"", ""fr"")"),"Structure du clan. Une bonne défense pour une base.")</f>
+        <v>Structure du clan. Une bonne défense pour une base.</v>
       </c>
       <c r="D417" s="23"/>
       <c r="E417" s="29"/>
       <c r="F417" s="23" t="s">
-        <v>1341</v>
+        <v>1337</v>
       </c>
       <c r="G417" s="29"/>
       <c r="H417" s="36"/>
       <c r="I417" s="29"/>
       <c r="J417" s="25" t="s">
-        <v>1342</v>
+        <v>1338</v>
       </c>
       <c r="K417" s="30"/>
       <c r="L417" s="35"/>
@@ -21682,25 +21686,25 @@
     </row>
     <row r="418">
       <c r="A418" s="41" t="s">
-        <v>1343</v>
+        <v>1339</v>
       </c>
       <c r="B418" s="22" t="s">
-        <v>1344</v>
+        <v>1340</v>
       </c>
       <c r="C418" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B418, ""en"", ""fr"")"),"Mur de fer")</f>
-        <v>Mur de fer</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B418, ""en"", ""fr"")"),"porte brique")</f>
+        <v>porte brique</v>
       </c>
       <c r="D418" s="23"/>
       <c r="E418" s="29"/>
       <c r="F418" s="23" t="s">
-        <v>1345</v>
+        <v>1341</v>
       </c>
       <c r="G418" s="29"/>
       <c r="H418" s="36"/>
       <c r="I418" s="29"/>
       <c r="J418" s="25" t="s">
-        <v>1346</v>
+        <v>1342</v>
       </c>
       <c r="K418" s="30"/>
       <c r="L418" s="35"/>
@@ -21723,25 +21727,25 @@
     </row>
     <row r="419">
       <c r="A419" s="41" t="s">
-        <v>1347</v>
+        <v>1343</v>
       </c>
       <c r="B419" s="22" t="s">
-        <v>1348</v>
+        <v>1344</v>
       </c>
       <c r="C419" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B419, ""en"", ""fr"")"),"Structure du clan. Une grande défense pour une base.")</f>
-        <v>Structure du clan. Une grande défense pour une base.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B419, ""en"", ""fr"")"),"Structure du clan. Ne peut être ouvert par les membres du clan. Plus fort que une porte en bois.")</f>
+        <v>Structure du clan. Ne peut être ouvert par les membres du clan. Plus fort que une porte en bois.</v>
       </c>
       <c r="D419" s="23"/>
       <c r="E419" s="29"/>
       <c r="F419" s="23" t="s">
-        <v>1349</v>
+        <v>1345</v>
       </c>
       <c r="G419" s="29"/>
       <c r="H419" s="36"/>
       <c r="I419" s="29"/>
       <c r="J419" s="25" t="s">
-        <v>1350</v>
+        <v>1346</v>
       </c>
       <c r="K419" s="30"/>
       <c r="L419" s="35"/>
@@ -21764,25 +21768,25 @@
     </row>
     <row r="420">
       <c r="A420" s="41" t="s">
-        <v>1351</v>
+        <v>1347</v>
       </c>
       <c r="B420" s="22" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="C420" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B420, ""en"", ""fr"")"),"Porte en fer")</f>
-        <v>Porte en fer</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B420, ""en"", ""fr"")"),"Mur de fer")</f>
+        <v>Mur de fer</v>
       </c>
       <c r="D420" s="23"/>
       <c r="E420" s="29"/>
       <c r="F420" s="23" t="s">
-        <v>1353</v>
+        <v>1349</v>
       </c>
       <c r="G420" s="29"/>
       <c r="H420" s="36"/>
       <c r="I420" s="29"/>
       <c r="J420" s="25" t="s">
-        <v>1354</v>
+        <v>1350</v>
       </c>
       <c r="K420" s="30"/>
       <c r="L420" s="35"/>
@@ -21805,25 +21809,25 @@
     </row>
     <row r="421">
       <c r="A421" s="41" t="s">
-        <v>1355</v>
+        <v>1351</v>
       </c>
       <c r="B421" s="22" t="s">
-        <v>1356</v>
+        <v>1352</v>
       </c>
       <c r="C421" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B421, ""en"", ""fr"")"),"Structure du clan. Ne peut être ouvert par les membres du clan. Plus fort que la porte de briques.")</f>
-        <v>Structure du clan. Ne peut être ouvert par les membres du clan. Plus fort que la porte de briques.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B421, ""en"", ""fr"")"),"Structure du clan. Une grande défense pour une base.")</f>
+        <v>Structure du clan. Une grande défense pour une base.</v>
       </c>
       <c r="D421" s="23"/>
       <c r="E421" s="29"/>
       <c r="F421" s="23" t="s">
-        <v>1357</v>
+        <v>1353</v>
       </c>
       <c r="G421" s="29"/>
       <c r="H421" s="36"/>
       <c r="I421" s="29"/>
       <c r="J421" s="25" t="s">
-        <v>1358</v>
+        <v>1354</v>
       </c>
       <c r="K421" s="30"/>
       <c r="L421" s="35"/>
@@ -21845,26 +21849,26 @@
       <c r="AB421" s="28"/>
     </row>
     <row r="422">
-      <c r="A422" s="21" t="s">
-        <v>1359</v>
+      <c r="A422" s="41" t="s">
+        <v>1355</v>
       </c>
       <c r="B422" s="22" t="s">
-        <v>1360</v>
+        <v>1356</v>
       </c>
       <c r="C422" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B422, ""en"", ""fr"")"),"Banque poitrine")</f>
-        <v>Banque poitrine</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B422, ""en"", ""fr"")"),"Porte en fer")</f>
+        <v>Porte en fer</v>
       </c>
       <c r="D422" s="23"/>
       <c r="E422" s="29"/>
       <c r="F422" s="23" t="s">
-        <v>1361</v>
+        <v>1357</v>
       </c>
       <c r="G422" s="29"/>
       <c r="H422" s="36"/>
       <c r="I422" s="29"/>
       <c r="J422" s="25" t="s">
-        <v>1362</v>
+        <v>1358</v>
       </c>
       <c r="K422" s="30"/>
       <c r="L422" s="35"/>
@@ -21886,26 +21890,26 @@
       <c r="AB422" s="28"/>
     </row>
     <row r="423">
-      <c r="A423" s="21" t="s">
-        <v>1363</v>
+      <c r="A423" s="41" t="s">
+        <v>1359</v>
       </c>
       <c r="B423" s="22" t="s">
-        <v>1364</v>
+        <v>1360</v>
       </c>
       <c r="C423" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B423, ""en"", ""fr"")"),"Structure du clan. Permet d'accéder à votre stockage bancaire personnel.")</f>
-        <v>Structure du clan. Permet d'accéder à votre stockage bancaire personnel.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B423, ""en"", ""fr"")"),"Structure du clan. Ne peut être ouvert par les membres du clan. Plus fort que la porte de briques.")</f>
+        <v>Structure du clan. Ne peut être ouvert par les membres du clan. Plus fort que la porte de briques.</v>
       </c>
       <c r="D423" s="23"/>
       <c r="E423" s="29"/>
       <c r="F423" s="23" t="s">
-        <v>1365</v>
+        <v>1361</v>
       </c>
       <c r="G423" s="29"/>
       <c r="H423" s="36"/>
       <c r="I423" s="29"/>
       <c r="J423" s="25" t="s">
-        <v>1366</v>
+        <v>1362</v>
       </c>
       <c r="K423" s="30"/>
       <c r="L423" s="35"/>
@@ -21928,25 +21932,25 @@
     </row>
     <row r="424">
       <c r="A424" s="21" t="s">
-        <v>1367</v>
+        <v>1363</v>
       </c>
       <c r="B424" s="22" t="s">
-        <v>751</v>
+        <v>1364</v>
       </c>
       <c r="C424" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B424, ""en"", ""fr"")"),"Table de travail")</f>
-        <v>Table de travail</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B424, ""en"", ""fr"")"),"Banque poitrine")</f>
+        <v>Banque poitrine</v>
       </c>
       <c r="D424" s="23"/>
       <c r="E424" s="29"/>
       <c r="F424" s="23" t="s">
-        <v>753</v>
+        <v>1365</v>
       </c>
       <c r="G424" s="29"/>
       <c r="H424" s="36"/>
       <c r="I424" s="29"/>
       <c r="J424" s="25" t="s">
-        <v>1368</v>
+        <v>1366</v>
       </c>
       <c r="K424" s="30"/>
       <c r="L424" s="35"/>
@@ -21969,25 +21973,25 @@
     </row>
     <row r="425">
       <c r="A425" s="21" t="s">
-        <v>1369</v>
+        <v>1367</v>
       </c>
       <c r="B425" s="22" t="s">
-        <v>1370</v>
+        <v>1368</v>
       </c>
       <c r="C425" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B425, ""en"", ""fr"")"),"Structure du clan. Utilisé pour fabriquer divers objets.")</f>
-        <v>Structure du clan. Utilisé pour fabriquer divers objets.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B425, ""en"", ""fr"")"),"Structure du clan. Permet d'accéder à votre stockage bancaire personnel.")</f>
+        <v>Structure du clan. Permet d'accéder à votre stockage bancaire personnel.</v>
       </c>
       <c r="D425" s="23"/>
       <c r="E425" s="29"/>
       <c r="F425" s="23" t="s">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="G425" s="29"/>
       <c r="H425" s="36"/>
       <c r="I425" s="29"/>
       <c r="J425" s="25" t="s">
-        <v>1372</v>
+        <v>1370</v>
       </c>
       <c r="K425" s="30"/>
       <c r="L425" s="35"/>
@@ -22010,25 +22014,25 @@
     </row>
     <row r="426">
       <c r="A426" s="21" t="s">
-        <v>1373</v>
+        <v>1371</v>
       </c>
       <c r="B426" s="22" t="s">
-        <v>745</v>
+        <v>751</v>
       </c>
       <c r="C426" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B426, ""en"", ""fr"")"),"fourneau")</f>
-        <v>fourneau</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B426, ""en"", ""fr"")"),"Table de travail")</f>
+        <v>Table de travail</v>
       </c>
       <c r="D426" s="23"/>
       <c r="E426" s="29"/>
       <c r="F426" s="23" t="s">
-        <v>747</v>
+        <v>753</v>
       </c>
       <c r="G426" s="29"/>
       <c r="H426" s="36"/>
       <c r="I426" s="29"/>
       <c r="J426" s="25" t="s">
-        <v>1374</v>
+        <v>1372</v>
       </c>
       <c r="K426" s="30"/>
       <c r="L426" s="35"/>
@@ -22051,25 +22055,25 @@
     </row>
     <row r="427">
       <c r="A427" s="21" t="s">
-        <v>1375</v>
+        <v>1373</v>
       </c>
       <c r="B427" s="22" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="C427" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B427, ""en"", ""fr"")"),"Structure du clan. Utilisé pour transformer les minerais en barres métalliques.")</f>
-        <v>Structure du clan. Utilisé pour transformer les minerais en barres métalliques.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B427, ""en"", ""fr"")"),"Structure du clan. Utilisé pour fabriquer divers objets.")</f>
+        <v>Structure du clan. Utilisé pour fabriquer divers objets.</v>
       </c>
       <c r="D427" s="23"/>
       <c r="E427" s="29"/>
       <c r="F427" s="23" t="s">
-        <v>1377</v>
+        <v>1375</v>
       </c>
       <c r="G427" s="29"/>
       <c r="H427" s="36"/>
       <c r="I427" s="29"/>
       <c r="J427" s="25" t="s">
-        <v>1378</v>
+        <v>1376</v>
       </c>
       <c r="K427" s="30"/>
       <c r="L427" s="35"/>
@@ -22092,25 +22096,25 @@
     </row>
     <row r="428">
       <c r="A428" s="21" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="B428" s="22" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="C428" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B428, ""en"", ""fr"")"),"Enclume")</f>
-        <v>Enclume</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B428, ""en"", ""fr"")"),"fourneau")</f>
+        <v>fourneau</v>
       </c>
       <c r="D428" s="23"/>
       <c r="E428" s="29"/>
       <c r="F428" s="23" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="G428" s="29"/>
       <c r="H428" s="36"/>
       <c r="I428" s="29"/>
       <c r="J428" s="25" t="s">
-        <v>1380</v>
+        <v>1378</v>
       </c>
       <c r="K428" s="30"/>
       <c r="L428" s="35"/>
@@ -22133,25 +22137,25 @@
     </row>
     <row r="429">
       <c r="A429" s="21" t="s">
-        <v>1381</v>
+        <v>1379</v>
       </c>
       <c r="B429" s="22" t="s">
-        <v>1382</v>
+        <v>1380</v>
       </c>
       <c r="C429" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B429, ""en"", ""fr"")"),"Structure du clan. Utilisé pour les objets métalliques d'artisanat.")</f>
-        <v>Structure du clan. Utilisé pour les objets métalliques d'artisanat.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B429, ""en"", ""fr"")"),"Structure du clan. Utilisé pour transformer les minerais en barres métalliques.")</f>
+        <v>Structure du clan. Utilisé pour transformer les minerais en barres métalliques.</v>
       </c>
       <c r="D429" s="23"/>
       <c r="E429" s="29"/>
       <c r="F429" s="23" t="s">
-        <v>1383</v>
+        <v>1381</v>
       </c>
       <c r="G429" s="29"/>
       <c r="H429" s="36"/>
       <c r="I429" s="29"/>
       <c r="J429" s="25" t="s">
-        <v>1384</v>
+        <v>1382</v>
       </c>
       <c r="K429" s="30"/>
       <c r="L429" s="35"/>
@@ -22173,26 +22177,26 @@
       <c r="AB429" s="28"/>
     </row>
     <row r="430">
-      <c r="A430" s="41" t="s">
-        <v>1385</v>
+      <c r="A430" s="21" t="s">
+        <v>1383</v>
       </c>
       <c r="B430" s="22" t="s">
-        <v>748</v>
+        <v>742</v>
       </c>
       <c r="C430" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B430, ""en"", ""fr"")"),"Laboratoire")</f>
-        <v>Laboratoire</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B430, ""en"", ""fr"")"),"Enclume")</f>
+        <v>Enclume</v>
       </c>
       <c r="D430" s="23"/>
       <c r="E430" s="29"/>
       <c r="F430" s="23" t="s">
-        <v>1386</v>
+        <v>744</v>
       </c>
       <c r="G430" s="29"/>
       <c r="H430" s="36"/>
       <c r="I430" s="29"/>
       <c r="J430" s="25" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
       <c r="K430" s="30"/>
       <c r="L430" s="35"/>
@@ -22214,26 +22218,26 @@
       <c r="AB430" s="28"/>
     </row>
     <row r="431">
-      <c r="A431" s="41" t="s">
-        <v>1388</v>
+      <c r="A431" s="21" t="s">
+        <v>1385</v>
       </c>
       <c r="B431" s="22" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
       <c r="C431" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B431, ""en"", ""fr"")"),"Structure du clan. Utilisé pour les potions d'artisanat.")</f>
-        <v>Structure du clan. Utilisé pour les potions d'artisanat.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B431, ""en"", ""fr"")"),"Structure du clan. Utilisé pour les objets métalliques d'artisanat.")</f>
+        <v>Structure du clan. Utilisé pour les objets métalliques d'artisanat.</v>
       </c>
       <c r="D431" s="23"/>
       <c r="E431" s="29"/>
       <c r="F431" s="23" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="G431" s="29"/>
       <c r="H431" s="36"/>
       <c r="I431" s="29"/>
       <c r="J431" s="25" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
       <c r="K431" s="30"/>
       <c r="L431" s="35"/>
@@ -22256,25 +22260,25 @@
     </row>
     <row r="432">
       <c r="A432" s="41" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="B432" s="22" t="s">
-        <v>1393</v>
+        <v>748</v>
       </c>
       <c r="C432" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B432, ""en"", ""fr"")"),"Générateur")</f>
-        <v>Générateur</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B432, ""en"", ""fr"")"),"Laboratoire")</f>
+        <v>Laboratoire</v>
       </c>
       <c r="D432" s="23"/>
       <c r="E432" s="29"/>
       <c r="F432" s="23" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="G432" s="29"/>
       <c r="H432" s="36"/>
       <c r="I432" s="29"/>
       <c r="J432" s="25" t="s">
-        <v>1395</v>
+        <v>1391</v>
       </c>
       <c r="K432" s="30"/>
       <c r="L432" s="35"/>
@@ -22297,25 +22301,25 @@
     </row>
     <row r="433">
       <c r="A433" s="41" t="s">
-        <v>1396</v>
+        <v>1392</v>
       </c>
       <c r="B433" s="22" t="s">
-        <v>1397</v>
+        <v>1393</v>
       </c>
       <c r="C433" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B433, ""en"", ""fr"")"),"Structure du clan. La gloire des joueurs convertis en puissance qui peuvent être utilisés pour activer d'autres structures claniques qui nécessitent une alimentation, et peut protéger toutes les structures de clan des dommages.")</f>
-        <v>Structure du clan. La gloire des joueurs convertis en puissance qui peuvent être utilisés pour activer d'autres structures claniques qui nécessitent une alimentation, et peut protéger toutes les structures de clan des dommages.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B433, ""en"", ""fr"")"),"Structure du clan. Utilisé pour les potions d'artisanat.")</f>
+        <v>Structure du clan. Utilisé pour les potions d'artisanat.</v>
       </c>
       <c r="D433" s="23"/>
       <c r="E433" s="29"/>
       <c r="F433" s="23" t="s">
-        <v>1398</v>
+        <v>1394</v>
       </c>
       <c r="G433" s="29"/>
       <c r="H433" s="36"/>
       <c r="I433" s="29"/>
       <c r="J433" s="25" t="s">
-        <v>1399</v>
+        <v>1395</v>
       </c>
       <c r="K433" s="30"/>
       <c r="L433" s="35"/>
@@ -22338,24 +22342,26 @@
     </row>
     <row r="434">
       <c r="A434" s="41" t="s">
-        <v>1400</v>
+        <v>1396</v>
       </c>
       <c r="B434" s="22" t="s">
-        <v>1401</v>
+        <v>1397</v>
       </c>
       <c r="C434" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B434, ""en"", ""fr"")"),"clé Fighter")</f>
-        <v>clé Fighter</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B434, ""en"", ""fr"")"),"Générateur")</f>
+        <v>Générateur</v>
       </c>
       <c r="D434" s="23"/>
       <c r="E434" s="29"/>
       <c r="F434" s="23" t="s">
-        <v>1402</v>
+        <v>1398</v>
       </c>
       <c r="G434" s="29"/>
       <c r="H434" s="36"/>
       <c r="I434" s="29"/>
-      <c r="J434" s="25"/>
+      <c r="J434" s="25" t="s">
+        <v>1399</v>
+      </c>
       <c r="K434" s="30"/>
       <c r="L434" s="35"/>
       <c r="M434" s="28"/>
@@ -22377,24 +22383,26 @@
     </row>
     <row r="435">
       <c r="A435" s="41" t="s">
-        <v>1403</v>
+        <v>1400</v>
       </c>
       <c r="B435" s="22" t="s">
-        <v>1404</v>
+        <v>1401</v>
       </c>
       <c r="C435" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B435, ""en"", ""fr"")"),"Ouvre la porte à la zone de préparation de l'arène PvP. Avertissement! D'autres joueurs peuvent vous attaquer dans la fosse de combat!")</f>
-        <v>Ouvre la porte à la zone de préparation de l'arène PvP. Avertissement! D'autres joueurs peuvent vous attaquer dans la fosse de combat!</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B435, ""en"", ""fr"")"),"Structure du clan. La gloire des joueurs convertis en puissance qui peuvent être utilisés pour activer d'autres structures claniques qui nécessitent une alimentation, et peut protéger toutes les structures de clan des dommages.")</f>
+        <v>Structure du clan. La gloire des joueurs convertis en puissance qui peuvent être utilisés pour activer d'autres structures claniques qui nécessitent une alimentation, et peut protéger toutes les structures de clan des dommages.</v>
       </c>
       <c r="D435" s="23"/>
       <c r="E435" s="29"/>
       <c r="F435" s="23" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="G435" s="29"/>
       <c r="H435" s="36"/>
       <c r="I435" s="29"/>
-      <c r="J435" s="25"/>
+      <c r="J435" s="25" t="s">
+        <v>1403</v>
+      </c>
       <c r="K435" s="30"/>
       <c r="L435" s="35"/>
       <c r="M435" s="28"/>
@@ -22416,19 +22424,19 @@
     </row>
     <row r="436">
       <c r="A436" s="41" t="s">
-        <v>1406</v>
+        <v>1404</v>
       </c>
       <c r="B436" s="22" t="s">
-        <v>1407</v>
+        <v>1405</v>
       </c>
       <c r="C436" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B436, ""en"", ""fr"")"),"clé Pit")</f>
-        <v>clé Pit</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B436, ""en"", ""fr"")"),"clé Fighter")</f>
+        <v>clé Fighter</v>
       </c>
       <c r="D436" s="23"/>
       <c r="E436" s="29"/>
       <c r="F436" s="23" t="s">
-        <v>1408</v>
+        <v>1406</v>
       </c>
       <c r="G436" s="29"/>
       <c r="H436" s="36"/>
@@ -22455,19 +22463,19 @@
     </row>
     <row r="437">
       <c r="A437" s="41" t="s">
-        <v>1409</v>
+        <v>1407</v>
       </c>
       <c r="B437" s="22" t="s">
-        <v>1410</v>
+        <v>1408</v>
       </c>
       <c r="C437" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B437, ""en"", ""fr"")"),"Ouvre les portes pour sortir de la fosse de combat.")</f>
-        <v>Ouvre les portes pour sortir de la fosse de combat.</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B437, ""en"", ""fr"")"),"Ouvre la porte à la zone de préparation de l'arène PvP. Avertissement! D'autres joueurs peuvent vous attaquer dans la fosse de combat!")</f>
+        <v>Ouvre la porte à la zone de préparation de l'arène PvP. Avertissement! D'autres joueurs peuvent vous attaquer dans la fosse de combat!</v>
       </c>
       <c r="D437" s="23"/>
       <c r="E437" s="29"/>
       <c r="F437" s="23" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="G437" s="29"/>
       <c r="H437" s="36"/>
@@ -22493,29 +22501,25 @@
       <c r="AB437" s="28"/>
     </row>
     <row r="438">
-      <c r="A438" s="21" t="s">
-        <v>1412</v>
+      <c r="A438" s="41" t="s">
+        <v>1410</v>
       </c>
       <c r="B438" s="22" t="s">
-        <v>1413</v>
+        <v>1411</v>
       </c>
       <c r="C438" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B438, ""en"", ""fr"")"),"Bandit")</f>
-        <v>Bandit</v>
-      </c>
-      <c r="D438" s="29"/>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B438, ""en"", ""fr"")"),"clé Pit")</f>
+        <v>clé Pit</v>
+      </c>
+      <c r="D438" s="23"/>
       <c r="E438" s="29"/>
       <c r="F438" s="23" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="G438" s="29"/>
       <c r="H438" s="36"/>
-      <c r="I438" s="23" t="s">
-        <v>1415</v>
-      </c>
-      <c r="J438" s="25" t="s">
-        <v>1416</v>
-      </c>
+      <c r="I438" s="29"/>
+      <c r="J438" s="25"/>
       <c r="K438" s="30"/>
       <c r="L438" s="35"/>
       <c r="M438" s="28"/>
@@ -22536,27 +22540,25 @@
       <c r="AB438" s="28"/>
     </row>
     <row r="439">
-      <c r="A439" s="21" t="s">
-        <v>1417</v>
+      <c r="A439" s="41" t="s">
+        <v>1413</v>
       </c>
       <c r="B439" s="22" t="s">
-        <v>1418</v>
+        <v>1414</v>
       </c>
       <c r="C439" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B439, ""en"", ""fr"")"),"Bandit leader")</f>
-        <v>Bandit leader</v>
-      </c>
-      <c r="D439" s="29"/>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B439, ""en"", ""fr"")"),"Ouvre les portes pour sortir de la fosse de combat.")</f>
+        <v>Ouvre les portes pour sortir de la fosse de combat.</v>
+      </c>
+      <c r="D439" s="23"/>
       <c r="E439" s="29"/>
       <c r="F439" s="23" t="s">
-        <v>1419</v>
+        <v>1415</v>
       </c>
       <c r="G439" s="29"/>
       <c r="H439" s="36"/>
       <c r="I439" s="29"/>
-      <c r="J439" s="25" t="s">
-        <v>1420</v>
-      </c>
+      <c r="J439" s="25"/>
       <c r="K439" s="30"/>
       <c r="L439" s="35"/>
       <c r="M439" s="28"/>
@@ -22578,25 +22580,27 @@
     </row>
     <row r="440">
       <c r="A440" s="21" t="s">
-        <v>1421</v>
+        <v>1416</v>
       </c>
       <c r="B440" s="22" t="s">
-        <v>1422</v>
+        <v>1417</v>
       </c>
       <c r="C440" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B440, ""en"", ""fr"")"),"Assassin")</f>
-        <v>Assassin</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B440, ""en"", ""fr"")"),"Bandit")</f>
+        <v>Bandit</v>
       </c>
       <c r="D440" s="29"/>
       <c r="E440" s="29"/>
       <c r="F440" s="23" t="s">
-        <v>1423</v>
+        <v>1418</v>
       </c>
       <c r="G440" s="29"/>
       <c r="H440" s="36"/>
-      <c r="I440" s="29"/>
+      <c r="I440" s="23" t="s">
+        <v>1419</v>
+      </c>
       <c r="J440" s="25" t="s">
-        <v>1424</v>
+        <v>1420</v>
       </c>
       <c r="K440" s="30"/>
       <c r="L440" s="35"/>
@@ -22619,24 +22623,26 @@
     </row>
     <row r="441">
       <c r="A441" s="21" t="s">
-        <v>1425</v>
+        <v>1421</v>
       </c>
       <c r="B441" s="22" t="s">
-        <v>1426</v>
+        <v>1422</v>
       </c>
       <c r="C441" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B441, ""en"", ""fr"")"),"maître assassin")</f>
-        <v>maître assassin</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B441, ""en"", ""fr"")"),"Bandit leader")</f>
+        <v>Bandit leader</v>
       </c>
       <c r="D441" s="29"/>
       <c r="E441" s="29"/>
       <c r="F441" s="23" t="s">
-        <v>1427</v>
+        <v>1423</v>
       </c>
       <c r="G441" s="29"/>
       <c r="H441" s="36"/>
       <c r="I441" s="29"/>
-      <c r="J441" s="25"/>
+      <c r="J441" s="25" t="s">
+        <v>1424</v>
+      </c>
       <c r="K441" s="30"/>
       <c r="L441" s="35"/>
       <c r="M441" s="28"/>
@@ -22658,27 +22664,25 @@
     </row>
     <row r="442">
       <c r="A442" s="21" t="s">
-        <v>1428</v>
+        <v>1425</v>
       </c>
       <c r="B442" s="22" t="s">
-        <v>1429</v>
+        <v>1426</v>
       </c>
       <c r="C442" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B442, ""en"", ""fr"")"),"Chauve souris")</f>
-        <v>Chauve souris</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B442, ""en"", ""fr"")"),"Assassin")</f>
+        <v>Assassin</v>
       </c>
       <c r="D442" s="29"/>
       <c r="E442" s="29"/>
       <c r="F442" s="23" t="s">
-        <v>1430</v>
+        <v>1427</v>
       </c>
       <c r="G442" s="29"/>
       <c r="H442" s="36"/>
-      <c r="I442" s="23" t="s">
-        <v>1431</v>
-      </c>
+      <c r="I442" s="29"/>
       <c r="J442" s="25" t="s">
-        <v>1432</v>
+        <v>1428</v>
       </c>
       <c r="K442" s="30"/>
       <c r="L442" s="35"/>
@@ -22701,26 +22705,24 @@
     </row>
     <row r="443">
       <c r="A443" s="21" t="s">
-        <v>1433</v>
+        <v>1429</v>
       </c>
       <c r="B443" s="22" t="s">
-        <v>1434</v>
+        <v>1430</v>
       </c>
       <c r="C443" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B443, ""en"", ""fr"")"),"Règle")</f>
-        <v>Règle</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B443, ""en"", ""fr"")"),"maître assassin")</f>
+        <v>maître assassin</v>
       </c>
       <c r="D443" s="29"/>
       <c r="E443" s="29"/>
       <c r="F443" s="23" t="s">
-        <v>1435</v>
+        <v>1431</v>
       </c>
       <c r="G443" s="29"/>
       <c r="H443" s="36"/>
       <c r="I443" s="29"/>
-      <c r="J443" s="25" t="s">
-        <v>1436</v>
-      </c>
+      <c r="J443" s="25"/>
       <c r="K443" s="30"/>
       <c r="L443" s="35"/>
       <c r="M443" s="28"/>
@@ -22742,25 +22744,27 @@
     </row>
     <row r="444">
       <c r="A444" s="21" t="s">
-        <v>1437</v>
+        <v>1432</v>
       </c>
       <c r="B444" s="22" t="s">
-        <v>1438</v>
+        <v>1433</v>
       </c>
       <c r="C444" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B444, ""en"", ""fr"")"),"Aubergiste")</f>
-        <v>Aubergiste</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B444, ""en"", ""fr"")"),"Chauve souris")</f>
+        <v>Chauve souris</v>
       </c>
       <c r="D444" s="29"/>
       <c r="E444" s="29"/>
       <c r="F444" s="23" t="s">
-        <v>1439</v>
+        <v>1434</v>
       </c>
       <c r="G444" s="29"/>
       <c r="H444" s="36"/>
-      <c r="I444" s="29"/>
+      <c r="I444" s="23" t="s">
+        <v>1435</v>
+      </c>
       <c r="J444" s="25" t="s">
-        <v>1440</v>
+        <v>1436</v>
       </c>
       <c r="K444" s="30"/>
       <c r="L444" s="35"/>
@@ -22783,24 +22787,26 @@
     </row>
     <row r="445">
       <c r="A445" s="21" t="s">
-        <v>1441</v>
+        <v>1437</v>
       </c>
       <c r="B445" s="22" t="s">
-        <v>1442</v>
+        <v>1438</v>
       </c>
       <c r="C445" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B445, ""en"", ""fr"")"),"maître Arena")</f>
-        <v>maître Arena</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B445, ""en"", ""fr"")"),"Règle")</f>
+        <v>Règle</v>
       </c>
       <c r="D445" s="29"/>
       <c r="E445" s="29"/>
       <c r="F445" s="23" t="s">
-        <v>1443</v>
+        <v>1439</v>
       </c>
       <c r="G445" s="29"/>
       <c r="H445" s="36"/>
       <c r="I445" s="29"/>
-      <c r="J445" s="25"/>
+      <c r="J445" s="25" t="s">
+        <v>1440</v>
+      </c>
       <c r="K445" s="30"/>
       <c r="L445" s="35"/>
       <c r="M445" s="28"/>
@@ -22822,27 +22828,25 @@
     </row>
     <row r="446">
       <c r="A446" s="21" t="s">
-        <v>1444</v>
+        <v>1441</v>
       </c>
       <c r="B446" s="22" t="s">
-        <v>1445</v>
+        <v>1442</v>
       </c>
       <c r="C446" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B446, ""en"", ""fr"")"),"marchande")</f>
-        <v>marchande</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B446, ""en"", ""fr"")"),"Aubergiste")</f>
+        <v>Aubergiste</v>
       </c>
       <c r="D446" s="29"/>
       <c r="E446" s="29"/>
       <c r="F446" s="23" t="s">
-        <v>1446</v>
+        <v>1443</v>
       </c>
       <c r="G446" s="29"/>
       <c r="H446" s="36"/>
-      <c r="I446" s="23" t="s">
-        <v>1447</v>
-      </c>
+      <c r="I446" s="29"/>
       <c r="J446" s="25" t="s">
-        <v>1448</v>
+        <v>1444</v>
       </c>
       <c r="K446" s="30"/>
       <c r="L446" s="35"/>
@@ -22865,26 +22869,24 @@
     </row>
     <row r="447">
       <c r="A447" s="21" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="B447" s="22" t="s">
-        <v>1450</v>
+        <v>1446</v>
       </c>
       <c r="C447" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B447, ""en"", ""fr"")"),"marchand Melee")</f>
-        <v>marchand Melee</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B447, ""en"", ""fr"")"),"maître Arena")</f>
+        <v>maître Arena</v>
       </c>
       <c r="D447" s="29"/>
       <c r="E447" s="29"/>
       <c r="F447" s="23" t="s">
-        <v>1451</v>
+        <v>1447</v>
       </c>
       <c r="G447" s="29"/>
       <c r="H447" s="36"/>
       <c r="I447" s="29"/>
-      <c r="J447" s="25" t="s">
-        <v>1452</v>
-      </c>
+      <c r="J447" s="25"/>
       <c r="K447" s="30"/>
       <c r="L447" s="35"/>
       <c r="M447" s="28"/>
@@ -22906,25 +22908,27 @@
     </row>
     <row r="448">
       <c r="A448" s="21" t="s">
-        <v>1453</v>
+        <v>1448</v>
       </c>
       <c r="B448" s="22" t="s">
-        <v>1454</v>
+        <v>1449</v>
       </c>
       <c r="C448" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B448, ""en"", ""fr"")"),"marchand Ranged")</f>
-        <v>marchand Ranged</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B448, ""en"", ""fr"")"),"marchande")</f>
+        <v>marchande</v>
       </c>
       <c r="D448" s="29"/>
       <c r="E448" s="29"/>
       <c r="F448" s="23" t="s">
-        <v>1455</v>
+        <v>1450</v>
       </c>
       <c r="G448" s="29"/>
       <c r="H448" s="36"/>
-      <c r="I448" s="29"/>
+      <c r="I448" s="23" t="s">
+        <v>1451</v>
+      </c>
       <c r="J448" s="25" t="s">
-        <v>1456</v>
+        <v>1452</v>
       </c>
       <c r="K448" s="30"/>
       <c r="L448" s="35"/>
@@ -22947,25 +22951,25 @@
     </row>
     <row r="449">
       <c r="A449" s="21" t="s">
-        <v>1457</v>
+        <v>1453</v>
       </c>
       <c r="B449" s="22" t="s">
-        <v>1458</v>
+        <v>1454</v>
       </c>
       <c r="C449" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B449, ""en"", ""fr"")"),"marchand magique")</f>
-        <v>marchand magique</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B449, ""en"", ""fr"")"),"marchand Melee")</f>
+        <v>marchand Melee</v>
       </c>
       <c r="D449" s="29"/>
       <c r="E449" s="29"/>
       <c r="F449" s="23" t="s">
-        <v>1459</v>
+        <v>1455</v>
       </c>
       <c r="G449" s="29"/>
       <c r="H449" s="36"/>
       <c r="I449" s="29"/>
       <c r="J449" s="25" t="s">
-        <v>1460</v>
+        <v>1456</v>
       </c>
       <c r="K449" s="30"/>
       <c r="L449" s="35"/>
@@ -22988,25 +22992,25 @@
     </row>
     <row r="450">
       <c r="A450" s="21" t="s">
-        <v>1461</v>
+        <v>1457</v>
       </c>
       <c r="B450" s="22" t="s">
-        <v>1462</v>
+        <v>1458</v>
       </c>
       <c r="C450" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B450, ""en"", ""fr"")"),"marchand outil")</f>
-        <v>marchand outil</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B450, ""en"", ""fr"")"),"marchand Ranged")</f>
+        <v>marchand Ranged</v>
       </c>
       <c r="D450" s="29"/>
       <c r="E450" s="29"/>
       <c r="F450" s="23" t="s">
-        <v>1463</v>
+        <v>1459</v>
       </c>
       <c r="G450" s="29"/>
       <c r="H450" s="36"/>
       <c r="I450" s="29"/>
       <c r="J450" s="25" t="s">
-        <v>1464</v>
+        <v>1460</v>
       </c>
       <c r="K450" s="30"/>
       <c r="L450" s="35"/>
@@ -23029,24 +23033,26 @@
     </row>
     <row r="451">
       <c r="A451" s="21" t="s">
-        <v>1465</v>
+        <v>1461</v>
       </c>
       <c r="B451" s="22" t="s">
-        <v>1466</v>
+        <v>1462</v>
       </c>
       <c r="C451" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B451, ""en"", ""fr"")"),"marchand nain")</f>
-        <v>marchand nain</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B451, ""en"", ""fr"")"),"marchand magique")</f>
+        <v>marchand magique</v>
       </c>
       <c r="D451" s="29"/>
       <c r="E451" s="29"/>
       <c r="F451" s="23" t="s">
-        <v>1467</v>
+        <v>1463</v>
       </c>
       <c r="G451" s="29"/>
       <c r="H451" s="36"/>
       <c r="I451" s="29"/>
-      <c r="J451" s="25"/>
+      <c r="J451" s="25" t="s">
+        <v>1464</v>
+      </c>
       <c r="K451" s="30"/>
       <c r="L451" s="35"/>
       <c r="M451" s="28"/>
@@ -23068,24 +23074,26 @@
     </row>
     <row r="452">
       <c r="A452" s="21" t="s">
-        <v>1468</v>
+        <v>1465</v>
       </c>
       <c r="B452" s="22" t="s">
-        <v>1469</v>
+        <v>1466</v>
       </c>
       <c r="C452" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B452, ""en"", ""fr"")"),"Bibliothécaire")</f>
-        <v>Bibliothécaire</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B452, ""en"", ""fr"")"),"marchand outil")</f>
+        <v>marchand outil</v>
       </c>
       <c r="D452" s="29"/>
       <c r="E452" s="29"/>
       <c r="F452" s="23" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
       <c r="G452" s="29"/>
       <c r="H452" s="36"/>
       <c r="I452" s="29"/>
-      <c r="J452" s="25"/>
+      <c r="J452" s="25" t="s">
+        <v>1468</v>
+      </c>
       <c r="K452" s="30"/>
       <c r="L452" s="35"/>
       <c r="M452" s="28"/>
@@ -23107,18 +23115,20 @@
     </row>
     <row r="453">
       <c r="A453" s="21" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="B453" s="22" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="C453" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B453, ""en"", ""fr"")"),"Omni marchand")</f>
-        <v>Omni marchand</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B453, ""en"", ""fr"")"),"marchand nain")</f>
+        <v>marchand nain</v>
       </c>
       <c r="D453" s="29"/>
       <c r="E453" s="29"/>
-      <c r="F453" s="23"/>
+      <c r="F453" s="23" t="s">
+        <v>1471</v>
+      </c>
       <c r="G453" s="29"/>
       <c r="H453" s="36"/>
       <c r="I453" s="29"/>
@@ -23144,26 +23154,24 @@
     </row>
     <row r="454">
       <c r="A454" s="21" t="s">
+        <v>1472</v>
+      </c>
+      <c r="B454" s="22" t="s">
         <v>1473</v>
       </c>
-      <c r="B454" s="22" t="s">
-        <v>1474</v>
-      </c>
       <c r="C454" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B454, ""en"", ""fr"")"),"Prêtre")</f>
-        <v>Prêtre</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B454, ""en"", ""fr"")"),"Bibliothécaire")</f>
+        <v>Bibliothécaire</v>
       </c>
       <c r="D454" s="29"/>
       <c r="E454" s="29"/>
       <c r="F454" s="23" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="G454" s="29"/>
       <c r="H454" s="36"/>
       <c r="I454" s="29"/>
-      <c r="J454" s="25" t="s">
-        <v>1476</v>
-      </c>
+      <c r="J454" s="25"/>
       <c r="K454" s="30"/>
       <c r="L454" s="35"/>
       <c r="M454" s="28"/>
@@ -23185,26 +23193,22 @@
     </row>
     <row r="455">
       <c r="A455" s="21" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
       <c r="B455" s="22" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="C455" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B455, ""en"", ""fr"")"),"Citoyenne")</f>
-        <v>Citoyenne</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B455, ""en"", ""fr"")"),"Omni marchand")</f>
+        <v>Omni marchand</v>
       </c>
       <c r="D455" s="29"/>
       <c r="E455" s="29"/>
-      <c r="F455" s="23" t="s">
-        <v>1479</v>
-      </c>
+      <c r="F455" s="23"/>
       <c r="G455" s="29"/>
       <c r="H455" s="36"/>
       <c r="I455" s="29"/>
-      <c r="J455" s="25" t="s">
-        <v>1480</v>
-      </c>
+      <c r="J455" s="25"/>
       <c r="K455" s="30"/>
       <c r="L455" s="35"/>
       <c r="M455" s="28"/>
@@ -23226,22 +23230,26 @@
     </row>
     <row r="456">
       <c r="A456" s="21" t="s">
-        <v>1481</v>
+        <v>1477</v>
       </c>
       <c r="B456" s="22" t="s">
-        <v>1482</v>
+        <v>1478</v>
       </c>
       <c r="C456" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B456, ""en"", ""fr"")"),"Nain")</f>
-        <v>Nain</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B456, ""en"", ""fr"")"),"Prêtre")</f>
+        <v>Prêtre</v>
       </c>
       <c r="D456" s="29"/>
       <c r="E456" s="29"/>
-      <c r="F456" s="23"/>
+      <c r="F456" s="23" t="s">
+        <v>1479</v>
+      </c>
       <c r="G456" s="29"/>
       <c r="H456" s="36"/>
       <c r="I456" s="29"/>
-      <c r="J456" s="25"/>
+      <c r="J456" s="25" t="s">
+        <v>1480</v>
+      </c>
       <c r="K456" s="30"/>
       <c r="L456" s="35"/>
       <c r="M456" s="28"/>
@@ -23263,22 +23271,26 @@
     </row>
     <row r="457">
       <c r="A457" s="21" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="B457" s="22" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="C457" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B457, ""en"", ""fr"")"),"guerrier nain")</f>
-        <v>guerrier nain</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B457, ""en"", ""fr"")"),"Citoyenne")</f>
+        <v>Citoyenne</v>
       </c>
       <c r="D457" s="29"/>
       <c r="E457" s="29"/>
-      <c r="F457" s="23"/>
+      <c r="F457" s="23" t="s">
+        <v>1483</v>
+      </c>
       <c r="G457" s="29"/>
       <c r="H457" s="36"/>
       <c r="I457" s="29"/>
-      <c r="J457" s="25"/>
+      <c r="J457" s="25" t="s">
+        <v>1484</v>
+      </c>
       <c r="K457" s="30"/>
       <c r="L457" s="35"/>
       <c r="M457" s="28"/>
@@ -23306,22 +23318,16 @@
         <v>1486</v>
       </c>
       <c r="C458" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B458, ""en"", ""fr"")"),"chevalier")</f>
-        <v>chevalier</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B458, ""en"", ""fr"")"),"Nain")</f>
+        <v>Nain</v>
       </c>
       <c r="D458" s="29"/>
       <c r="E458" s="29"/>
-      <c r="F458" s="23" t="s">
-        <v>1487</v>
-      </c>
+      <c r="F458" s="23"/>
       <c r="G458" s="29"/>
       <c r="H458" s="36"/>
-      <c r="I458" s="23" t="s">
-        <v>1488</v>
-      </c>
-      <c r="J458" s="25" t="s">
-        <v>1489</v>
-      </c>
+      <c r="I458" s="29"/>
+      <c r="J458" s="25"/>
       <c r="K458" s="30"/>
       <c r="L458" s="35"/>
       <c r="M458" s="28"/>
@@ -23343,28 +23349,22 @@
     </row>
     <row r="459">
       <c r="A459" s="21" t="s">
-        <v>1490</v>
+        <v>1487</v>
       </c>
       <c r="B459" s="22" t="s">
-        <v>1491</v>
+        <v>1488</v>
       </c>
       <c r="C459" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B459, ""en"", ""fr"")"),"Le commandant")</f>
-        <v>Le commandant</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B459, ""en"", ""fr"")"),"guerrier nain")</f>
+        <v>guerrier nain</v>
       </c>
       <c r="D459" s="29"/>
       <c r="E459" s="29"/>
-      <c r="F459" s="23" t="s">
-        <v>1492</v>
-      </c>
+      <c r="F459" s="23"/>
       <c r="G459" s="29"/>
       <c r="H459" s="36"/>
-      <c r="I459" s="23" t="s">
-        <v>1493</v>
-      </c>
-      <c r="J459" s="25" t="s">
-        <v>1494</v>
-      </c>
+      <c r="I459" s="29"/>
+      <c r="J459" s="25"/>
       <c r="K459" s="30"/>
       <c r="L459" s="35"/>
       <c r="M459" s="28"/>
@@ -23386,27 +23386,27 @@
     </row>
     <row r="460">
       <c r="A460" s="21" t="s">
-        <v>1495</v>
+        <v>1489</v>
       </c>
       <c r="B460" s="22" t="s">
-        <v>1496</v>
+        <v>1490</v>
       </c>
       <c r="C460" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B460, ""en"", ""fr"")"),"guerrier")</f>
-        <v>guerrier</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B460, ""en"", ""fr"")"),"chevalier")</f>
+        <v>chevalier</v>
       </c>
       <c r="D460" s="29"/>
       <c r="E460" s="29"/>
       <c r="F460" s="23" t="s">
-        <v>1497</v>
+        <v>1491</v>
       </c>
       <c r="G460" s="29"/>
       <c r="H460" s="36"/>
       <c r="I460" s="23" t="s">
-        <v>1498</v>
+        <v>1492</v>
       </c>
       <c r="J460" s="25" t="s">
-        <v>1499</v>
+        <v>1493</v>
       </c>
       <c r="K460" s="30"/>
       <c r="L460" s="35"/>
@@ -23429,27 +23429,27 @@
     </row>
     <row r="461">
       <c r="A461" s="21" t="s">
-        <v>1500</v>
+        <v>1494</v>
       </c>
       <c r="B461" s="22" t="s">
-        <v>1501</v>
+        <v>1495</v>
       </c>
       <c r="C461" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B461, ""en"", ""fr"")"),"Prisonnier")</f>
-        <v>Prisonnier</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B461, ""en"", ""fr"")"),"Le commandant")</f>
+        <v>Le commandant</v>
       </c>
       <c r="D461" s="29"/>
       <c r="E461" s="29"/>
       <c r="F461" s="23" t="s">
-        <v>1502</v>
+        <v>1496</v>
       </c>
       <c r="G461" s="29"/>
       <c r="H461" s="36"/>
       <c r="I461" s="23" t="s">
-        <v>1503</v>
+        <v>1497</v>
       </c>
       <c r="J461" s="25" t="s">
-        <v>1504</v>
+        <v>1498</v>
       </c>
       <c r="K461" s="30"/>
       <c r="L461" s="35"/>
@@ -23472,27 +23472,27 @@
     </row>
     <row r="462">
       <c r="A462" s="21" t="s">
-        <v>1505</v>
+        <v>1499</v>
       </c>
       <c r="B462" s="22" t="s">
-        <v>1506</v>
+        <v>1500</v>
       </c>
       <c r="C462" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B462, ""en"", ""fr"")"),"Rat")</f>
-        <v>Rat</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B462, ""en"", ""fr"")"),"guerrier")</f>
+        <v>guerrier</v>
       </c>
       <c r="D462" s="29"/>
       <c r="E462" s="29"/>
       <c r="F462" s="23" t="s">
-        <v>1507</v>
+        <v>1501</v>
       </c>
       <c r="G462" s="29"/>
       <c r="H462" s="36"/>
       <c r="I462" s="23" t="s">
-        <v>1508</v>
+        <v>1502</v>
       </c>
       <c r="J462" s="25" t="s">
-        <v>1509</v>
+        <v>1503</v>
       </c>
       <c r="K462" s="30"/>
       <c r="L462" s="35"/>
@@ -23515,25 +23515,27 @@
     </row>
     <row r="463">
       <c r="A463" s="21" t="s">
-        <v>1510</v>
+        <v>1504</v>
       </c>
       <c r="B463" s="22" t="s">
-        <v>1511</v>
+        <v>1505</v>
       </c>
       <c r="C463" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B463, ""en"", ""fr"")"),"faucon")</f>
-        <v>faucon</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B463, ""en"", ""fr"")"),"Prisonnier")</f>
+        <v>Prisonnier</v>
       </c>
       <c r="D463" s="29"/>
       <c r="E463" s="29"/>
       <c r="F463" s="23" t="s">
-        <v>1512</v>
+        <v>1506</v>
       </c>
       <c r="G463" s="29"/>
       <c r="H463" s="36"/>
-      <c r="I463" s="29"/>
+      <c r="I463" s="23" t="s">
+        <v>1507</v>
+      </c>
       <c r="J463" s="25" t="s">
-        <v>1513</v>
+        <v>1508</v>
       </c>
       <c r="K463" s="30"/>
       <c r="L463" s="35"/>
@@ -23556,25 +23558,27 @@
     </row>
     <row r="464">
       <c r="A464" s="21" t="s">
-        <v>1514</v>
+        <v>1509</v>
       </c>
       <c r="B464" s="22" t="s">
-        <v>1515</v>
+        <v>1510</v>
       </c>
       <c r="C464" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B464, ""en"", ""fr"")"),"vaurien de sable")</f>
-        <v>vaurien de sable</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B464, ""en"", ""fr"")"),"Rat")</f>
+        <v>Rat</v>
       </c>
       <c r="D464" s="29"/>
       <c r="E464" s="29"/>
       <c r="F464" s="23" t="s">
-        <v>1516</v>
+        <v>1511</v>
       </c>
       <c r="G464" s="29"/>
       <c r="H464" s="36"/>
-      <c r="I464" s="29"/>
+      <c r="I464" s="23" t="s">
+        <v>1512</v>
+      </c>
       <c r="J464" s="25" t="s">
-        <v>1517</v>
+        <v>1513</v>
       </c>
       <c r="K464" s="30"/>
       <c r="L464" s="35"/>
@@ -23597,24 +23601,26 @@
     </row>
     <row r="465">
       <c r="A465" s="21" t="s">
-        <v>1518</v>
+        <v>1514</v>
       </c>
       <c r="B465" s="22" t="s">
-        <v>1519</v>
+        <v>1515</v>
       </c>
       <c r="C465" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B465, ""en"", ""fr"")"),"herbe vaurien")</f>
-        <v>herbe vaurien</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B465, ""en"", ""fr"")"),"faucon")</f>
+        <v>faucon</v>
       </c>
       <c r="D465" s="29"/>
       <c r="E465" s="29"/>
       <c r="F465" s="23" t="s">
-        <v>1520</v>
+        <v>1516</v>
       </c>
       <c r="G465" s="29"/>
       <c r="H465" s="36"/>
       <c r="I465" s="29"/>
-      <c r="J465" s="25"/>
+      <c r="J465" s="25" t="s">
+        <v>1517</v>
+      </c>
       <c r="K465" s="30"/>
       <c r="L465" s="35"/>
       <c r="M465" s="28"/>
@@ -23636,27 +23642,25 @@
     </row>
     <row r="466">
       <c r="A466" s="21" t="s">
-        <v>1521</v>
+        <v>1518</v>
       </c>
       <c r="B466" s="22" t="s">
-        <v>1522</v>
+        <v>1519</v>
       </c>
       <c r="C466" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B466, ""en"", ""fr"")"),"Lutin")</f>
-        <v>Lutin</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B466, ""en"", ""fr"")"),"vaurien de sable")</f>
+        <v>vaurien de sable</v>
       </c>
       <c r="D466" s="29"/>
       <c r="E466" s="29"/>
       <c r="F466" s="23" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="G466" s="29"/>
       <c r="H466" s="36"/>
-      <c r="I466" s="23" t="s">
-        <v>1522</v>
-      </c>
+      <c r="I466" s="29"/>
       <c r="J466" s="25" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="K466" s="30"/>
       <c r="L466" s="35"/>
@@ -23679,28 +23683,24 @@
     </row>
     <row r="467">
       <c r="A467" s="21" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="B467" s="22" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="C467" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B467, ""en"", ""fr"")"),"Druide")</f>
-        <v>Druide</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B467, ""en"", ""fr"")"),"herbe vaurien")</f>
+        <v>herbe vaurien</v>
       </c>
       <c r="D467" s="29"/>
       <c r="E467" s="29"/>
       <c r="F467" s="23" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
       <c r="G467" s="29"/>
       <c r="H467" s="36"/>
-      <c r="I467" s="23" t="s">
-        <v>1525</v>
-      </c>
-      <c r="J467" s="25" t="s">
-        <v>1527</v>
-      </c>
+      <c r="I467" s="29"/>
+      <c r="J467" s="25"/>
       <c r="K467" s="30"/>
       <c r="L467" s="35"/>
       <c r="M467" s="28"/>
@@ -23722,25 +23722,27 @@
     </row>
     <row r="468">
       <c r="A468" s="21" t="s">
-        <v>1528</v>
+        <v>1525</v>
       </c>
       <c r="B468" s="22" t="s">
-        <v>1529</v>
+        <v>1526</v>
       </c>
       <c r="C468" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B468, ""en"", ""fr"")"),"Snoovir")</f>
-        <v>Snoovir</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B468, ""en"", ""fr"")"),"Lutin")</f>
+        <v>Lutin</v>
       </c>
       <c r="D468" s="29"/>
       <c r="E468" s="29"/>
       <c r="F468" s="23" t="s">
-        <v>1530</v>
+        <v>1526</v>
       </c>
       <c r="G468" s="29"/>
       <c r="H468" s="36"/>
-      <c r="I468" s="29"/>
+      <c r="I468" s="23" t="s">
+        <v>1526</v>
+      </c>
       <c r="J468" s="25" t="s">
-        <v>1531</v>
+        <v>1527</v>
       </c>
       <c r="K468" s="30"/>
       <c r="L468" s="35"/>
@@ -23763,27 +23765,27 @@
     </row>
     <row r="469">
       <c r="A469" s="21" t="s">
-        <v>1532</v>
+        <v>1528</v>
       </c>
       <c r="B469" s="22" t="s">
-        <v>1533</v>
+        <v>1529</v>
       </c>
       <c r="C469" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B469, ""en"", ""fr"")"),"Zombi")</f>
-        <v>Zombi</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B469, ""en"", ""fr"")"),"Druide")</f>
+        <v>Druide</v>
       </c>
       <c r="D469" s="29"/>
       <c r="E469" s="29"/>
       <c r="F469" s="23" t="s">
-        <v>1534</v>
+        <v>1530</v>
       </c>
       <c r="G469" s="29"/>
       <c r="H469" s="36"/>
       <c r="I469" s="23" t="s">
-        <v>1534</v>
+        <v>1529</v>
       </c>
       <c r="J469" s="25" t="s">
-        <v>1535</v>
+        <v>1531</v>
       </c>
       <c r="K469" s="30"/>
       <c r="L469" s="35"/>
@@ -23806,27 +23808,25 @@
     </row>
     <row r="470">
       <c r="A470" s="21" t="s">
-        <v>1536</v>
+        <v>1532</v>
       </c>
       <c r="B470" s="22" t="s">
-        <v>1537</v>
+        <v>1533</v>
       </c>
       <c r="C470" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B470, ""en"", ""fr"")"),"Momie")</f>
-        <v>Momie</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B470, ""en"", ""fr"")"),"Snoovir")</f>
+        <v>Snoovir</v>
       </c>
       <c r="D470" s="29"/>
       <c r="E470" s="29"/>
       <c r="F470" s="23" t="s">
-        <v>1538</v>
+        <v>1534</v>
       </c>
       <c r="G470" s="29"/>
       <c r="H470" s="36"/>
-      <c r="I470" s="23" t="s">
-        <v>1539</v>
-      </c>
+      <c r="I470" s="29"/>
       <c r="J470" s="25" t="s">
-        <v>1540</v>
+        <v>1535</v>
       </c>
       <c r="K470" s="30"/>
       <c r="L470" s="35"/>
@@ -23849,25 +23849,27 @@
     </row>
     <row r="471">
       <c r="A471" s="21" t="s">
-        <v>1541</v>
+        <v>1536</v>
       </c>
       <c r="B471" s="22" t="s">
-        <v>1542</v>
+        <v>1537</v>
       </c>
       <c r="C471" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B471, ""en"", ""fr"")"),"gardien crypte")</f>
-        <v>gardien crypte</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B471, ""en"", ""fr"")"),"Zombi")</f>
+        <v>Zombi</v>
       </c>
       <c r="D471" s="29"/>
       <c r="E471" s="29"/>
       <c r="F471" s="23" t="s">
-        <v>1543</v>
+        <v>1538</v>
       </c>
       <c r="G471" s="29"/>
       <c r="H471" s="36"/>
-      <c r="I471" s="29"/>
+      <c r="I471" s="23" t="s">
+        <v>1538</v>
+      </c>
       <c r="J471" s="25" t="s">
-        <v>1544</v>
+        <v>1539</v>
       </c>
       <c r="K471" s="30"/>
       <c r="L471" s="35"/>
@@ -23890,27 +23892,27 @@
     </row>
     <row r="472">
       <c r="A472" s="21" t="s">
-        <v>1545</v>
+        <v>1540</v>
       </c>
       <c r="B472" s="22" t="s">
-        <v>1546</v>
+        <v>1541</v>
       </c>
       <c r="C472" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B472, ""en"", ""fr"")"),"pharaon")</f>
-        <v>pharaon</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B472, ""en"", ""fr"")"),"Momie")</f>
+        <v>Momie</v>
       </c>
       <c r="D472" s="29"/>
       <c r="E472" s="29"/>
       <c r="F472" s="23" t="s">
-        <v>1547</v>
+        <v>1542</v>
       </c>
       <c r="G472" s="29"/>
       <c r="H472" s="36"/>
       <c r="I472" s="23" t="s">
-        <v>1548</v>
+        <v>1543</v>
       </c>
       <c r="J472" s="25" t="s">
-        <v>1549</v>
+        <v>1544</v>
       </c>
       <c r="K472" s="30"/>
       <c r="L472" s="35"/>
@@ -23933,25 +23935,25 @@
     </row>
     <row r="473">
       <c r="A473" s="21" t="s">
-        <v>1550</v>
+        <v>1545</v>
       </c>
       <c r="B473" s="22" t="s">
-        <v>1551</v>
+        <v>1546</v>
       </c>
       <c r="C473" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B473, ""en"", ""fr"")"),"Vampire")</f>
-        <v>Vampire</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B473, ""en"", ""fr"")"),"gardien crypte")</f>
+        <v>gardien crypte</v>
       </c>
       <c r="D473" s="29"/>
       <c r="E473" s="29"/>
       <c r="F473" s="23" t="s">
-        <v>1552</v>
+        <v>1547</v>
       </c>
       <c r="G473" s="29"/>
       <c r="H473" s="36"/>
       <c r="I473" s="29"/>
       <c r="J473" s="25" t="s">
-        <v>1553</v>
+        <v>1548</v>
       </c>
       <c r="K473" s="30"/>
       <c r="L473" s="35"/>
@@ -23974,27 +23976,27 @@
     </row>
     <row r="474">
       <c r="A474" s="21" t="s">
-        <v>1554</v>
+        <v>1549</v>
       </c>
       <c r="B474" s="22" t="s">
-        <v>1555</v>
+        <v>1550</v>
       </c>
       <c r="C474" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B474, ""en"", ""fr"")"),"prêtre de sang")</f>
-        <v>prêtre de sang</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B474, ""en"", ""fr"")"),"pharaon")</f>
+        <v>pharaon</v>
       </c>
       <c r="D474" s="29"/>
       <c r="E474" s="29"/>
       <c r="F474" s="23" t="s">
-        <v>1556</v>
+        <v>1551</v>
       </c>
       <c r="G474" s="29"/>
       <c r="H474" s="36"/>
       <c r="I474" s="23" t="s">
-        <v>1557</v>
+        <v>1552</v>
       </c>
       <c r="J474" s="25" t="s">
-        <v>1558</v>
+        <v>1553</v>
       </c>
       <c r="K474" s="30"/>
       <c r="L474" s="35"/>
@@ -24017,25 +24019,25 @@
     </row>
     <row r="475">
       <c r="A475" s="21" t="s">
-        <v>1559</v>
+        <v>1554</v>
       </c>
       <c r="B475" s="22" t="s">
-        <v>1560</v>
+        <v>1555</v>
       </c>
       <c r="C475" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B475, ""en"", ""fr"")"),"seigneur de sang")</f>
-        <v>seigneur de sang</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B475, ""en"", ""fr"")"),"Vampire")</f>
+        <v>Vampire</v>
       </c>
       <c r="D475" s="29"/>
       <c r="E475" s="29"/>
       <c r="F475" s="23" t="s">
-        <v>1561</v>
+        <v>1556</v>
       </c>
       <c r="G475" s="29"/>
       <c r="H475" s="36"/>
       <c r="I475" s="29"/>
       <c r="J475" s="25" t="s">
-        <v>1562</v>
+        <v>1557</v>
       </c>
       <c r="K475" s="30"/>
       <c r="L475" s="35"/>
@@ -24058,23 +24060,28 @@
     </row>
     <row r="476">
       <c r="A476" s="21" t="s">
-        <v>1563</v>
+        <v>1558</v>
       </c>
       <c r="B476" s="22" t="s">
-        <v>1564</v>
-      </c>
-      <c r="C476" s="23" t="s">
-        <v>1564</v>
+        <v>1559</v>
+      </c>
+      <c r="C476" s="23" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B476, ""en"", ""fr"")"),"prêtre de sang")</f>
+        <v>prêtre de sang</v>
       </c>
       <c r="D476" s="29"/>
       <c r="E476" s="29"/>
       <c r="F476" s="23" t="s">
-        <v>1565</v>
+        <v>1560</v>
       </c>
       <c r="G476" s="29"/>
       <c r="H476" s="36"/>
-      <c r="I476" s="29"/>
-      <c r="J476" s="30"/>
+      <c r="I476" s="23" t="s">
+        <v>1561</v>
+      </c>
+      <c r="J476" s="25" t="s">
+        <v>1562</v>
+      </c>
       <c r="K476" s="30"/>
       <c r="L476" s="35"/>
       <c r="M476" s="28"/>
@@ -24096,24 +24103,26 @@
     </row>
     <row r="477">
       <c r="A477" s="21" t="s">
-        <v>1566</v>
+        <v>1563</v>
       </c>
       <c r="B477" s="22" t="s">
-        <v>1567</v>
+        <v>1564</v>
       </c>
       <c r="C477" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B477, ""en"", ""fr"")"),"grande gnarl")</f>
-        <v>grande gnarl</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B477, ""en"", ""fr"")"),"seigneur de sang")</f>
+        <v>seigneur de sang</v>
       </c>
       <c r="D477" s="29"/>
       <c r="E477" s="29"/>
       <c r="F477" s="23" t="s">
-        <v>1568</v>
+        <v>1565</v>
       </c>
       <c r="G477" s="29"/>
       <c r="H477" s="36"/>
       <c r="I477" s="29"/>
-      <c r="J477" s="30"/>
+      <c r="J477" s="25" t="s">
+        <v>1566</v>
+      </c>
       <c r="K477" s="30"/>
       <c r="L477" s="35"/>
       <c r="M477" s="28"/>
@@ -24135,19 +24144,18 @@
     </row>
     <row r="478">
       <c r="A478" s="21" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="B478" s="22" t="s">
-        <v>1570</v>
-      </c>
-      <c r="C478" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B478, ""en"", ""fr"")"),"mage")</f>
-        <v>mage</v>
+        <v>1568</v>
+      </c>
+      <c r="C478" s="23" t="s">
+        <v>1568</v>
       </c>
       <c r="D478" s="29"/>
       <c r="E478" s="29"/>
       <c r="F478" s="23" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="G478" s="29"/>
       <c r="H478" s="36"/>
@@ -24174,19 +24182,19 @@
     </row>
     <row r="479">
       <c r="A479" s="21" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="B479" s="22" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
       <c r="C479" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B479, ""en"", ""fr"")"),"arc mage")</f>
-        <v>arc mage</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B479, ""en"", ""fr"")"),"grande gnarl")</f>
+        <v>grande gnarl</v>
       </c>
       <c r="D479" s="29"/>
       <c r="E479" s="29"/>
       <c r="F479" s="23" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
       <c r="G479" s="29"/>
       <c r="H479" s="36"/>
@@ -24213,18 +24221,20 @@
     </row>
     <row r="480">
       <c r="A480" s="21" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
       <c r="B480" s="22" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
       <c r="C480" s="23" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B480, ""en"", ""fr"")"),"adumbral")</f>
-        <v>adumbral</v>
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B480, ""en"", ""fr"")"),"mage")</f>
+        <v>mage</v>
       </c>
       <c r="D480" s="29"/>
       <c r="E480" s="29"/>
-      <c r="F480" s="29"/>
+      <c r="F480" s="23" t="s">
+        <v>1575</v>
+      </c>
       <c r="G480" s="29"/>
       <c r="H480" s="36"/>
       <c r="I480" s="29"/>
@@ -24249,12 +24259,21 @@
       <c r="AB480" s="28"/>
     </row>
     <row r="481">
-      <c r="A481" s="42"/>
-      <c r="B481" s="43"/>
-      <c r="C481" s="29"/>
+      <c r="A481" s="21" t="s">
+        <v>1576</v>
+      </c>
+      <c r="B481" s="22" t="s">
+        <v>1577</v>
+      </c>
+      <c r="C481" s="23" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B481, ""en"", ""fr"")"),"arc mage")</f>
+        <v>arc mage</v>
+      </c>
       <c r="D481" s="29"/>
       <c r="E481" s="29"/>
-      <c r="F481" s="29"/>
+      <c r="F481" s="23" t="s">
+        <v>1578</v>
+      </c>
       <c r="G481" s="29"/>
       <c r="H481" s="36"/>
       <c r="I481" s="29"/>
@@ -24279,9 +24298,16 @@
       <c r="AB481" s="28"/>
     </row>
     <row r="482">
-      <c r="A482" s="42"/>
-      <c r="B482" s="43"/>
-      <c r="C482" s="29"/>
+      <c r="A482" s="21" t="s">
+        <v>1579</v>
+      </c>
+      <c r="B482" s="22" t="s">
+        <v>1580</v>
+      </c>
+      <c r="C482" s="23" t="str">
+        <f>IFERROR(__xludf.DUMMYFUNCTION("GOOGLETRANSLATE(B482, ""en"", ""fr"")"),"adumbral")</f>
+        <v>adumbral</v>
+      </c>
       <c r="D482" s="29"/>
       <c r="E482" s="29"/>
       <c r="F482" s="29"/>
@@ -26019,64 +26045,64 @@
       <c r="AB539" s="28"/>
     </row>
     <row r="540">
-      <c r="A540" s="1"/>
-      <c r="B540" s="44"/>
-      <c r="C540" s="44"/>
-      <c r="D540" s="44"/>
-      <c r="E540" s="44"/>
-      <c r="F540" s="44"/>
-      <c r="G540" s="44"/>
-      <c r="H540" s="45"/>
-      <c r="I540" s="44"/>
-      <c r="J540" s="46"/>
-      <c r="K540" s="46"/>
-      <c r="L540" s="47"/>
-      <c r="M540" s="47"/>
-      <c r="N540" s="47"/>
-      <c r="O540" s="47"/>
-      <c r="P540" s="47"/>
-      <c r="Q540" s="47"/>
-      <c r="R540" s="47"/>
-      <c r="S540" s="47"/>
-      <c r="T540" s="47"/>
-      <c r="U540" s="47"/>
-      <c r="V540" s="47"/>
-      <c r="W540" s="47"/>
-      <c r="X540" s="47"/>
-      <c r="Y540" s="47"/>
-      <c r="Z540" s="47"/>
-      <c r="AA540" s="47"/>
-      <c r="AB540" s="47"/>
+      <c r="A540" s="42"/>
+      <c r="B540" s="43"/>
+      <c r="C540" s="29"/>
+      <c r="D540" s="29"/>
+      <c r="E540" s="29"/>
+      <c r="F540" s="29"/>
+      <c r="G540" s="29"/>
+      <c r="H540" s="36"/>
+      <c r="I540" s="29"/>
+      <c r="J540" s="30"/>
+      <c r="K540" s="30"/>
+      <c r="L540" s="35"/>
+      <c r="M540" s="28"/>
+      <c r="N540" s="28"/>
+      <c r="O540" s="28"/>
+      <c r="P540" s="28"/>
+      <c r="Q540" s="28"/>
+      <c r="R540" s="28"/>
+      <c r="S540" s="28"/>
+      <c r="T540" s="28"/>
+      <c r="U540" s="28"/>
+      <c r="V540" s="28"/>
+      <c r="W540" s="28"/>
+      <c r="X540" s="28"/>
+      <c r="Y540" s="28"/>
+      <c r="Z540" s="28"/>
+      <c r="AA540" s="28"/>
+      <c r="AB540" s="28"/>
     </row>
     <row r="541">
-      <c r="A541" s="1"/>
-      <c r="B541" s="44"/>
-      <c r="C541" s="44"/>
-      <c r="D541" s="44"/>
-      <c r="E541" s="44"/>
-      <c r="F541" s="44"/>
-      <c r="G541" s="44"/>
-      <c r="H541" s="45"/>
-      <c r="I541" s="44"/>
-      <c r="J541" s="46"/>
-      <c r="K541" s="46"/>
-      <c r="L541" s="47"/>
-      <c r="M541" s="47"/>
-      <c r="N541" s="47"/>
-      <c r="O541" s="47"/>
-      <c r="P541" s="47"/>
-      <c r="Q541" s="47"/>
-      <c r="R541" s="47"/>
-      <c r="S541" s="47"/>
-      <c r="T541" s="47"/>
-      <c r="U541" s="47"/>
-      <c r="V541" s="47"/>
-      <c r="W541" s="47"/>
-      <c r="X541" s="47"/>
-      <c r="Y541" s="47"/>
-      <c r="Z541" s="47"/>
-      <c r="AA541" s="47"/>
-      <c r="AB541" s="47"/>
+      <c r="A541" s="42"/>
+      <c r="B541" s="43"/>
+      <c r="C541" s="29"/>
+      <c r="D541" s="29"/>
+      <c r="E541" s="29"/>
+      <c r="F541" s="29"/>
+      <c r="G541" s="29"/>
+      <c r="H541" s="36"/>
+      <c r="I541" s="29"/>
+      <c r="J541" s="30"/>
+      <c r="K541" s="30"/>
+      <c r="L541" s="35"/>
+      <c r="M541" s="28"/>
+      <c r="N541" s="28"/>
+      <c r="O541" s="28"/>
+      <c r="P541" s="28"/>
+      <c r="Q541" s="28"/>
+      <c r="R541" s="28"/>
+      <c r="S541" s="28"/>
+      <c r="T541" s="28"/>
+      <c r="U541" s="28"/>
+      <c r="V541" s="28"/>
+      <c r="W541" s="28"/>
+      <c r="X541" s="28"/>
+      <c r="Y541" s="28"/>
+      <c r="Z541" s="28"/>
+      <c r="AA541" s="28"/>
+      <c r="AB541" s="28"/>
     </row>
     <row r="542">
       <c r="A542" s="1"/>
@@ -53288,6 +53314,66 @@
       <c r="AA1448" s="47"/>
       <c r="AB1448" s="47"/>
     </row>
+    <row r="1449">
+      <c r="A1449" s="1"/>
+      <c r="B1449" s="44"/>
+      <c r="C1449" s="44"/>
+      <c r="D1449" s="44"/>
+      <c r="E1449" s="44"/>
+      <c r="F1449" s="44"/>
+      <c r="G1449" s="44"/>
+      <c r="H1449" s="45"/>
+      <c r="I1449" s="44"/>
+      <c r="J1449" s="46"/>
+      <c r="K1449" s="46"/>
+      <c r="L1449" s="47"/>
+      <c r="M1449" s="47"/>
+      <c r="N1449" s="47"/>
+      <c r="O1449" s="47"/>
+      <c r="P1449" s="47"/>
+      <c r="Q1449" s="47"/>
+      <c r="R1449" s="47"/>
+      <c r="S1449" s="47"/>
+      <c r="T1449" s="47"/>
+      <c r="U1449" s="47"/>
+      <c r="V1449" s="47"/>
+      <c r="W1449" s="47"/>
+      <c r="X1449" s="47"/>
+      <c r="Y1449" s="47"/>
+      <c r="Z1449" s="47"/>
+      <c r="AA1449" s="47"/>
+      <c r="AB1449" s="47"/>
+    </row>
+    <row r="1450">
+      <c r="A1450" s="1"/>
+      <c r="B1450" s="44"/>
+      <c r="C1450" s="44"/>
+      <c r="D1450" s="44"/>
+      <c r="E1450" s="44"/>
+      <c r="F1450" s="44"/>
+      <c r="G1450" s="44"/>
+      <c r="H1450" s="45"/>
+      <c r="I1450" s="44"/>
+      <c r="J1450" s="46"/>
+      <c r="K1450" s="46"/>
+      <c r="L1450" s="47"/>
+      <c r="M1450" s="47"/>
+      <c r="N1450" s="47"/>
+      <c r="O1450" s="47"/>
+      <c r="P1450" s="47"/>
+      <c r="Q1450" s="47"/>
+      <c r="R1450" s="47"/>
+      <c r="S1450" s="47"/>
+      <c r="T1450" s="47"/>
+      <c r="U1450" s="47"/>
+      <c r="V1450" s="47"/>
+      <c r="W1450" s="47"/>
+      <c r="X1450" s="47"/>
+      <c r="Y1450" s="47"/>
+      <c r="Z1450" s="47"/>
+      <c r="AA1450" s="47"/>
+      <c r="AB1450" s="47"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>